<commit_message>
Tana outlet locations sensor sites for 2022
</commit_message>
<xml_diff>
--- a/data/subcatchments_metadata/Subcatchments_existing_data_metadata.xlsx
+++ b/data/subcatchments_metadata/Subcatchments_existing_data_metadata.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="K:\Avdeling\317 Klima- og miljømodellering\LJB\Projects\Quantom\Data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Data\GitHub\quantom\data\subcatchments_metadata\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9CC71FEC-BAF7-4917-8F42-40174B891A42}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{76E9B92D-9504-4152-AFCD-84BAF44EE767}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17640" activeTab="6" xr2:uid="{3F73A599-D124-4158-BF3B-2BBEA0E40BC3}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17640" activeTab="5" xr2:uid="{3F73A599-D124-4158-BF3B-2BBEA0E40BC3}"/>
   </bookViews>
   <sheets>
     <sheet name="Hydrol" sheetId="1" r:id="rId1"/>
@@ -1089,7 +1089,7 @@
   <dimension ref="A1:Y14"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="R14" sqref="R14"/>
+      <selection activeCell="D3" sqref="D3:X3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -3304,7 +3304,7 @@
   <dimension ref="A1:I32"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B9" sqref="B9:H14"/>
+      <selection activeCell="D2" sqref="D2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -3323,10 +3323,10 @@
         <v>21</v>
       </c>
       <c r="D1" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="E1" s="1" t="s">
         <v>22</v>
-      </c>
-      <c r="E1" s="1" t="s">
-        <v>23</v>
       </c>
       <c r="F1" s="1" t="s">
         <v>113</v>
@@ -3693,10 +3693,10 @@
         <v>149</v>
       </c>
       <c r="D15" s="6">
+        <v>25.780663164598501</v>
+      </c>
+      <c r="E15" s="6">
         <v>69.35282494184429</v>
-      </c>
-      <c r="E15" s="6">
-        <v>25.780663164598501</v>
       </c>
       <c r="F15" s="6" t="s">
         <v>150</v>
@@ -3719,10 +3719,10 @@
         <v>149</v>
       </c>
       <c r="D16" s="6">
+        <v>25.21361834597635</v>
+      </c>
+      <c r="E16" s="6">
         <v>69.443804309461029</v>
-      </c>
-      <c r="E16" s="6">
-        <v>25.21361834597635</v>
       </c>
       <c r="F16" s="6" t="s">
         <v>150</v>
@@ -3745,10 +3745,10 @@
         <v>149</v>
       </c>
       <c r="D17" s="6">
+        <v>25.691932628253909</v>
+      </c>
+      <c r="E17" s="6">
         <v>69.442455747083997</v>
-      </c>
-      <c r="E17" s="6">
-        <v>25.691932628253909</v>
       </c>
       <c r="F17" s="6" t="s">
         <v>150</v>
@@ -3771,10 +3771,10 @@
         <v>149</v>
       </c>
       <c r="D18" s="6">
+        <v>27.121354681470969</v>
+      </c>
+      <c r="E18" s="6">
         <v>69.927720542756759</v>
-      </c>
-      <c r="E18" s="6">
-        <v>27.121354681470969</v>
       </c>
       <c r="F18" s="6" t="s">
         <v>150</v>
@@ -3797,10 +3797,10 @@
         <v>149</v>
       </c>
       <c r="D19" s="6">
+        <v>25.85313273161557</v>
+      </c>
+      <c r="E19" s="6">
         <v>69.472572555143302</v>
-      </c>
-      <c r="E19" s="6">
-        <v>25.85313273161557</v>
       </c>
       <c r="F19" s="6" t="s">
         <v>150</v>
@@ -3823,10 +3823,10 @@
         <v>149</v>
       </c>
       <c r="D20" s="6">
+        <v>28.19830818020764</v>
+      </c>
+      <c r="E20" s="6">
         <v>70.195935132530565</v>
-      </c>
-      <c r="E20" s="6">
-        <v>28.19830818020764</v>
       </c>
       <c r="F20" s="6" t="s">
         <v>150</v>
@@ -3849,10 +3849,10 @@
         <v>149</v>
       </c>
       <c r="D21" s="6">
+        <v>28.16908580439851</v>
+      </c>
+      <c r="E21" s="6">
         <v>70.22968067182029</v>
-      </c>
-      <c r="E21" s="6">
-        <v>28.16908580439851</v>
       </c>
       <c r="F21" s="6" t="s">
         <v>150</v>
@@ -3875,10 +3875,10 @@
         <v>149</v>
       </c>
       <c r="D22" s="6">
+        <v>27.720222929469681</v>
+      </c>
+      <c r="E22" s="6">
         <v>70.069685304299611</v>
-      </c>
-      <c r="E22" s="6">
-        <v>27.720222929469681</v>
       </c>
       <c r="F22" s="6" t="s">
         <v>150</v>
@@ -3901,10 +3901,10 @@
         <v>149</v>
       </c>
       <c r="D23" s="6">
+        <v>27.03387805245907</v>
+      </c>
+      <c r="E23" s="6">
         <v>69.910494088438014</v>
-      </c>
-      <c r="E23" s="6">
-        <v>27.03387805245907</v>
       </c>
       <c r="F23" s="6" t="s">
         <v>150</v>
@@ -3927,10 +3927,10 @@
         <v>149</v>
       </c>
       <c r="D24" s="9">
+        <v>25.597493</v>
+      </c>
+      <c r="E24" s="9">
         <v>68.926158000000001</v>
-      </c>
-      <c r="E24" s="9">
-        <v>25.597493</v>
       </c>
       <c r="F24" s="9" t="s">
         <v>204</v>
@@ -3953,10 +3953,10 @@
         <v>149</v>
       </c>
       <c r="D25" s="9">
+        <v>26.862095</v>
+      </c>
+      <c r="E25" s="9">
         <v>69.958485800000005</v>
-      </c>
-      <c r="E25" s="9">
-        <v>26.862095</v>
       </c>
       <c r="F25" s="9" t="s">
         <v>204</v>
@@ -3979,10 +3979,10 @@
         <v>149</v>
       </c>
       <c r="D26" s="9">
+        <v>25.098504399999999</v>
+      </c>
+      <c r="E26" s="9">
         <v>69.338290299999997</v>
-      </c>
-      <c r="E26" s="9">
-        <v>25.098504399999999</v>
       </c>
       <c r="F26" s="9" t="s">
         <v>204</v>
@@ -4005,10 +4005,10 @@
         <v>149</v>
       </c>
       <c r="D27" s="9">
+        <v>25.7197402</v>
+      </c>
+      <c r="E27" s="9">
         <v>69.106753400000002</v>
-      </c>
-      <c r="E27" s="9">
-        <v>25.7197402</v>
       </c>
       <c r="F27" s="9" t="s">
         <v>204</v>
@@ -4031,10 +4031,10 @@
         <v>149</v>
       </c>
       <c r="D28" s="9">
+        <v>24.472635199999999</v>
+      </c>
+      <c r="E28" s="9">
         <v>69.38992184</v>
-      </c>
-      <c r="E28" s="9">
-        <v>24.472635199999999</v>
       </c>
       <c r="F28" s="9" t="s">
         <v>204</v>
@@ -4057,10 +4057,10 @@
         <v>149</v>
       </c>
       <c r="D29" s="9">
+        <v>25.689412659999999</v>
+      </c>
+      <c r="E29" s="9">
         <v>69.199913890000005</v>
-      </c>
-      <c r="E29" s="9">
-        <v>25.689412659999999</v>
       </c>
       <c r="F29" s="9" t="s">
         <v>204</v>
@@ -4083,10 +4083,10 @@
         <v>149</v>
       </c>
       <c r="D30" s="9">
+        <v>24.010010829999999</v>
+      </c>
+      <c r="E30" s="9">
         <v>69.327241860000001</v>
-      </c>
-      <c r="E30" s="9">
-        <v>24.010010829999999</v>
       </c>
       <c r="F30" s="9" t="s">
         <v>204</v>
@@ -4109,10 +4109,10 @@
         <v>149</v>
       </c>
       <c r="D31" s="9">
+        <v>24.890296469999999</v>
+      </c>
+      <c r="E31" s="9">
         <v>69.534884730000002</v>
-      </c>
-      <c r="E31" s="9">
-        <v>24.890296469999999</v>
       </c>
       <c r="F31" s="9" t="s">
         <v>204</v>
@@ -4135,10 +4135,10 @@
         <v>149</v>
       </c>
       <c r="D32" s="9">
+        <v>26.424932210000001</v>
+      </c>
+      <c r="E32" s="9">
         <v>69.967677710000004</v>
-      </c>
-      <c r="E32" s="9">
-        <v>26.424932210000001</v>
       </c>
       <c r="F32" s="9" t="s">
         <v>204</v>
@@ -4161,12 +4161,13 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D314672D-2E53-44A1-A414-C2D66B05C403}">
   <dimension ref="A1:E10"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C12" sqref="C12"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
+    <col min="2" max="2" width="24.85546875" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="10.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
@@ -4178,10 +4179,10 @@
         <v>208</v>
       </c>
       <c r="C1" s="1" t="s">
+        <v>206</v>
+      </c>
+      <c r="D1" s="1" t="s">
         <v>205</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>206</v>
       </c>
       <c r="E1" s="1" t="s">
         <v>113</v>
@@ -4314,10 +4315,10 @@
         <v>133</v>
       </c>
       <c r="C9" s="6">
+        <v>25.21361834597635</v>
+      </c>
+      <c r="D9" s="6">
         <v>69.443804309461029</v>
-      </c>
-      <c r="D9" s="6">
-        <v>25.21361834597635</v>
       </c>
       <c r="E9" s="6" t="s">
         <v>150</v>
@@ -4331,10 +4332,10 @@
         <v>135</v>
       </c>
       <c r="C10" s="6">
+        <v>25.691932628253909</v>
+      </c>
+      <c r="D10" s="6">
         <v>69.442455747083997</v>
-      </c>
-      <c r="D10" s="6">
-        <v>25.691932628253909</v>
       </c>
       <c r="E10" s="6" t="s">
         <v>150</v>
@@ -4349,7 +4350,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F44B3DCA-1A3A-4728-8AB1-DB26F1C63506}">
   <dimension ref="A1:B10"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B11" sqref="B11"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
NVE data download and plotting
</commit_message>
<xml_diff>
--- a/data/subcatchments_metadata/Subcatchments_existing_data_metadata.xlsx
+++ b/data/subcatchments_metadata/Subcatchments_existing_data_metadata.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Data\GitHub\quantom\data\subcatchments_metadata\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{76E9B92D-9504-4152-AFCD-84BAF44EE767}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C5E27497-9A01-4C5E-A1DA-A3EBA0F47707}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17640" activeTab="5" xr2:uid="{3F73A599-D124-4158-BF3B-2BBEA0E40BC3}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17640" activeTab="6" xr2:uid="{3F73A599-D124-4158-BF3B-2BBEA0E40BC3}"/>
   </bookViews>
   <sheets>
     <sheet name="Hydrol" sheetId="1" r:id="rId1"/>
@@ -19,7 +19,9 @@
     <sheet name="Other" sheetId="5" r:id="rId4"/>
     <sheet name="ShortList" sheetId="4" r:id="rId5"/>
     <sheet name="Summary_forJLG_01-2022" sheetId="6" r:id="rId6"/>
-    <sheet name="NVE_datadownload_01-2022" sheetId="7" r:id="rId7"/>
+    <sheet name="nve_discharge" sheetId="7" r:id="rId7"/>
+    <sheet name="nve_stage_only" sheetId="8" r:id="rId8"/>
+    <sheet name="nve_SS_1208-1200" sheetId="9" r:id="rId9"/>
   </sheets>
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Hydrol!$A$1:$Y$14</definedName>
@@ -42,7 +44,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="486" uniqueCount="211">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="504" uniqueCount="215">
   <si>
     <t>objektType</t>
   </si>
@@ -675,6 +677,18 @@
   </si>
   <si>
     <t>Polmak</t>
+  </si>
+  <si>
+    <t>234.6.0</t>
+  </si>
+  <si>
+    <t>Vækkava</t>
+  </si>
+  <si>
+    <t>234.3.0</t>
+  </si>
+  <si>
+    <t>Jiesjavrre</t>
   </si>
 </sst>
 </file>
@@ -1089,14 +1103,16 @@
   <dimension ref="A1:Y14"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D3" sqref="D3:X3"/>
+      <selection activeCell="A14" sqref="A14:XFD14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="1" max="3" width="9.140625" style="1"/>
     <col min="4" max="4" width="19.140625" style="1" bestFit="1" customWidth="1"/>
-    <col min="5" max="15" width="9.140625" style="1"/>
+    <col min="5" max="5" width="9.140625" style="1"/>
+    <col min="6" max="6" width="15.85546875" style="1" customWidth="1"/>
+    <col min="7" max="15" width="9.140625" style="1"/>
     <col min="16" max="16" width="38.7109375" style="1" bestFit="1" customWidth="1"/>
     <col min="17" max="24" width="9.140625" style="1"/>
     <col min="25" max="25" width="129.7109375" style="1" bestFit="1" customWidth="1"/>
@@ -4161,7 +4177,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D314672D-2E53-44A1-A414-C2D66B05C403}">
   <dimension ref="A1:E10"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
@@ -4350,8 +4366,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F44B3DCA-1A3A-4728-8AB1-DB26F1C63506}">
   <dimension ref="A1:B10"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B11" sqref="B11"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="N28" sqref="N28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -4369,18 +4385,18 @@
     </row>
     <row r="2" spans="1:2">
       <c r="A2" t="s">
-        <v>57</v>
+        <v>26</v>
       </c>
       <c r="B2" t="s">
-        <v>58</v>
+        <v>27</v>
       </c>
     </row>
     <row r="3" spans="1:2">
       <c r="A3" t="s">
-        <v>26</v>
+        <v>36</v>
       </c>
       <c r="B3" t="s">
-        <v>27</v>
+        <v>37</v>
       </c>
     </row>
     <row r="4" spans="1:2">
@@ -4393,50 +4409,152 @@
     </row>
     <row r="5" spans="1:2">
       <c r="A5" t="s">
-        <v>36</v>
+        <v>209</v>
       </c>
       <c r="B5" t="s">
-        <v>37</v>
+        <v>210</v>
       </c>
     </row>
     <row r="6" spans="1:2">
       <c r="A6" t="s">
-        <v>52</v>
+        <v>48</v>
       </c>
       <c r="B6" t="s">
-        <v>53</v>
+        <v>49</v>
       </c>
     </row>
     <row r="7" spans="1:2">
       <c r="A7" t="s">
+        <v>52</v>
+      </c>
+      <c r="B7" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2">
+      <c r="A8" t="s">
+        <v>57</v>
+      </c>
+      <c r="B8" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2">
+      <c r="A9" t="s">
+        <v>211</v>
+      </c>
+      <c r="B9" t="s">
+        <v>212</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2">
+      <c r="A10" s="10" t="s">
+        <v>101</v>
+      </c>
+      <c r="B10" s="10" t="s">
+        <v>102</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DE091CD7-F5F7-4968-83AE-1EF24A409557}">
+  <dimension ref="A1:B4"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="L41" sqref="L41"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1" spans="1:2">
+      <c r="A1" t="s">
+        <v>2</v>
+      </c>
+      <c r="B1" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2">
+      <c r="A2" t="s">
         <v>66</v>
       </c>
-      <c r="B7" t="s">
+      <c r="B2" t="s">
         <v>67</v>
       </c>
     </row>
-    <row r="8" spans="1:2">
-      <c r="A8" s="10" t="s">
+    <row r="3" spans="1:2">
+      <c r="A3" t="s">
+        <v>79</v>
+      </c>
+      <c r="B3" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2">
+      <c r="A4" t="s">
+        <v>213</v>
+      </c>
+      <c r="B4" t="s">
+        <v>214</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{858FC109-75A4-4A0F-98BD-10924DC874B0}">
+  <dimension ref="A1:B5"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="R36" sqref="R36"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1" spans="1:2">
+      <c r="A1" t="s">
+        <v>2</v>
+      </c>
+      <c r="B1" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2">
+      <c r="A2" t="s">
+        <v>209</v>
+      </c>
+      <c r="B2" t="s">
+        <v>210</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2">
+      <c r="A3" t="s">
+        <v>48</v>
+      </c>
+      <c r="B3" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2">
+      <c r="A4" t="s">
+        <v>107</v>
+      </c>
+      <c r="B4" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2">
+      <c r="A5" s="10" t="s">
         <v>101</v>
       </c>
-      <c r="B8" s="10" t="s">
+      <c r="B5" s="10" t="s">
         <v>102</v>
-      </c>
-    </row>
-    <row r="9" spans="1:2">
-      <c r="A9" s="1" t="s">
-        <v>48</v>
-      </c>
-      <c r="B9" s="1" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="10" spans="1:2">
-      <c r="A10" t="s">
-        <v>209</v>
-      </c>
-      <c r="B10" t="s">
-        <v>210</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
First go at summary of points for delineating subcatchments in Tana
Based on location of monitoring points of interest (water chem, NVE, quantom, NoLa) plus manual amalgamation and some extras (e.g. large lake outflows).
</commit_message>
<xml_diff>
--- a/data/subcatchments_metadata/Subcatchments_existing_data_metadata.xlsx
+++ b/data/subcatchments_metadata/Subcatchments_existing_data_metadata.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Data\GitHub\quantom\data\subcatchments_metadata\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B352E49A-B33C-43BF-861C-D64170072E33}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A0D2A7BB-28A5-4FC8-BDB2-F54B0CF41F19}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17640" activeTab="5" xr2:uid="{3F73A599-D124-4158-BF3B-2BBEA0E40BC3}"/>
   </bookViews>
@@ -19,11 +19,13 @@
     <sheet name="quantom_2022_sensors" sheetId="13" r:id="rId4"/>
     <sheet name="Manual_SC_points" sheetId="12" r:id="rId5"/>
     <sheet name="Summary_all_points" sheetId="4" r:id="rId6"/>
+    <sheet name="Sheet1" sheetId="14" r:id="rId7"/>
   </sheets>
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Hydrol!$A$1:$E$14</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="2" hidden="1">Quantom_SCs!$A$1:$J$22</definedName>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="5" hidden="1">Summary_all_points!$A$1:$G$32</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="6" hidden="1">Sheet1!$A$1:$AB$35</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="5" hidden="1">Summary_all_points!$A$1:$F$36</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -41,7 +43,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="786" uniqueCount="265">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="951" uniqueCount="285">
   <si>
     <t>objektType</t>
   </si>
@@ -484,15 +486,9 @@
     <t>NVE</t>
   </si>
   <si>
-    <t>WGS84</t>
-  </si>
-  <si>
     <t>Vannmiljø</t>
   </si>
   <si>
-    <t>Get now?</t>
-  </si>
-  <si>
     <t>Just DS of confluence of Iesjohka and Karasjohka</t>
   </si>
   <si>
@@ -836,6 +832,72 @@
   </si>
   <si>
     <t>Tana_Polmak (NVE)</t>
+  </si>
+  <si>
+    <t>Long</t>
+  </si>
+  <si>
+    <t>Lat</t>
+  </si>
+  <si>
+    <t>Params</t>
+  </si>
+  <si>
+    <t>Groundwater level and temperature</t>
+  </si>
+  <si>
+    <t>Discharge</t>
+  </si>
+  <si>
+    <t>Discharge, SS</t>
+  </si>
+  <si>
+    <t>Soil temperature, soil moisture content, groundwater level, groundwater temperature</t>
+  </si>
+  <si>
+    <t>Stage</t>
+  </si>
+  <si>
+    <t>Snow depth</t>
+  </si>
+  <si>
+    <t>SS</t>
+  </si>
+  <si>
+    <t>Groundwater level</t>
+  </si>
+  <si>
+    <t>Water chem</t>
+  </si>
+  <si>
+    <t>Chem</t>
+  </si>
+  <si>
+    <t>Sensor</t>
+  </si>
+  <si>
+    <t>NVE, Quantom</t>
+  </si>
+  <si>
+    <t>Discharge, water temp (NVE), sensors (Quantom)</t>
+  </si>
+  <si>
+    <t>Sensor, discharge</t>
+  </si>
+  <si>
+    <t>Chem (Quantom), discharge and water temp (NVE)</t>
+  </si>
+  <si>
+    <t>Iesjohka_Veahkkava</t>
+  </si>
+  <si>
+    <t>Quantom, NVE</t>
+  </si>
+  <si>
+    <t>Karasjohka in town (NVE), M3</t>
+  </si>
+  <si>
+    <t>Discharge, water temp, SS (NVE), Sensor and chem (Quantom)</t>
   </si>
 </sst>
 </file>
@@ -845,7 +907,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="mmm\ dd\,\ yyyy"/>
   </numFmts>
-  <fonts count="11">
+  <fonts count="12">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -911,6 +973,14 @@
       <name val="Calibri"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -959,7 +1029,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="20">
+  <cellXfs count="26">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" applyFill="1"/>
@@ -996,6 +1066,22 @@
     </xf>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="2" fontId="11" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="2" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="2" fontId="1" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1314,7 +1400,7 @@
   <dimension ref="A1:AB35"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D33" sqref="D33"/>
+      <selection activeCell="A19" sqref="A19:XFD19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -1399,13 +1485,13 @@
         <v>23</v>
       </c>
       <c r="Y1" t="s">
-        <v>209</v>
+        <v>207</v>
       </c>
       <c r="Z1" t="s">
-        <v>236</v>
+        <v>234</v>
       </c>
       <c r="AA1" t="s">
-        <v>240</v>
+        <v>238</v>
       </c>
       <c r="AB1" t="s">
         <v>60</v>
@@ -1440,7 +1526,7 @@
         <v>29</v>
       </c>
       <c r="J2" t="s">
-        <v>214</v>
+        <v>212</v>
       </c>
       <c r="K2">
         <v>1</v>
@@ -1677,7 +1763,7 @@
         <v>2015</v>
       </c>
       <c r="G5" t="s">
-        <v>213</v>
+        <v>211</v>
       </c>
       <c r="H5">
         <v>1</v>
@@ -2004,7 +2090,7 @@
         <v>1200</v>
       </c>
       <c r="G9" s="8" t="s">
-        <v>217</v>
+        <v>215</v>
       </c>
       <c r="H9" s="8">
         <v>0</v>
@@ -2231,13 +2317,13 @@
         <v>24</v>
       </c>
       <c r="B12" t="s">
-        <v>227</v>
+        <v>225</v>
       </c>
       <c r="C12" t="s">
-        <v>203</v>
+        <v>201</v>
       </c>
       <c r="D12" t="s">
-        <v>204</v>
+        <v>202</v>
       </c>
       <c r="E12">
         <v>3</v>
@@ -2267,7 +2353,7 @@
         <v>30</v>
       </c>
       <c r="O12" t="s">
-        <v>210</v>
+        <v>208</v>
       </c>
       <c r="P12" t="s">
         <v>46</v>
@@ -2303,7 +2389,7 @@
         <v>0</v>
       </c>
       <c r="AB12" t="s">
-        <v>237</v>
+        <v>235</v>
       </c>
     </row>
     <row r="13" spans="1:28">
@@ -2311,13 +2397,13 @@
         <v>24</v>
       </c>
       <c r="B13" t="s">
-        <v>227</v>
+        <v>225</v>
       </c>
       <c r="C13" t="s">
-        <v>203</v>
+        <v>201</v>
       </c>
       <c r="D13" t="s">
-        <v>204</v>
+        <v>202</v>
       </c>
       <c r="E13">
         <v>3</v>
@@ -2326,7 +2412,7 @@
         <v>2015</v>
       </c>
       <c r="G13" t="s">
-        <v>213</v>
+        <v>211</v>
       </c>
       <c r="H13">
         <v>1</v>
@@ -2347,7 +2433,7 @@
         <v>30</v>
       </c>
       <c r="O13" t="s">
-        <v>210</v>
+        <v>208</v>
       </c>
       <c r="P13" t="s">
         <v>46</v>
@@ -2383,7 +2469,7 @@
         <v>0</v>
       </c>
       <c r="AB13" t="s">
-        <v>237</v>
+        <v>235</v>
       </c>
     </row>
     <row r="14" spans="1:28">
@@ -2391,13 +2477,13 @@
         <v>24</v>
       </c>
       <c r="B14" t="s">
-        <v>228</v>
+        <v>226</v>
       </c>
       <c r="C14" t="s">
-        <v>205</v>
+        <v>203</v>
       </c>
       <c r="D14" t="s">
-        <v>206</v>
+        <v>204</v>
       </c>
       <c r="E14">
         <v>3</v>
@@ -2427,7 +2513,7 @@
         <v>30</v>
       </c>
       <c r="O14" t="s">
-        <v>210</v>
+        <v>208</v>
       </c>
       <c r="P14" t="s">
         <v>46</v>
@@ -2463,7 +2549,7 @@
         <v>0</v>
       </c>
       <c r="AB14" t="s">
-        <v>237</v>
+        <v>235</v>
       </c>
     </row>
     <row r="15" spans="1:28">
@@ -2471,13 +2557,13 @@
         <v>24</v>
       </c>
       <c r="B15" t="s">
-        <v>229</v>
+        <v>227</v>
       </c>
       <c r="C15" t="s">
-        <v>207</v>
+        <v>205</v>
       </c>
       <c r="D15" t="s">
-        <v>208</v>
+        <v>206</v>
       </c>
       <c r="E15">
         <v>3</v>
@@ -2486,7 +2572,7 @@
         <v>2006</v>
       </c>
       <c r="G15" t="s">
-        <v>211</v>
+        <v>209</v>
       </c>
       <c r="H15">
         <v>1</v>
@@ -2495,7 +2581,7 @@
         <v>29</v>
       </c>
       <c r="J15" t="s">
-        <v>212</v>
+        <v>210</v>
       </c>
       <c r="K15">
         <v>1</v>
@@ -2510,7 +2596,7 @@
         <v>30</v>
       </c>
       <c r="O15" t="s">
-        <v>210</v>
+        <v>208</v>
       </c>
       <c r="P15" t="s">
         <v>46</v>
@@ -2546,7 +2632,7 @@
         <v>1</v>
       </c>
       <c r="AB15" t="s">
-        <v>237</v>
+        <v>235</v>
       </c>
     </row>
     <row r="16" spans="1:28">
@@ -2554,13 +2640,13 @@
         <v>24</v>
       </c>
       <c r="B16" t="s">
-        <v>229</v>
+        <v>227</v>
       </c>
       <c r="C16" t="s">
-        <v>207</v>
+        <v>205</v>
       </c>
       <c r="D16" t="s">
-        <v>208</v>
+        <v>206</v>
       </c>
       <c r="E16">
         <v>3</v>
@@ -2569,7 +2655,7 @@
         <v>2015</v>
       </c>
       <c r="G16" t="s">
-        <v>213</v>
+        <v>211</v>
       </c>
       <c r="H16">
         <v>1</v>
@@ -2593,7 +2679,7 @@
         <v>30</v>
       </c>
       <c r="O16" t="s">
-        <v>210</v>
+        <v>208</v>
       </c>
       <c r="P16" t="s">
         <v>46</v>
@@ -2629,7 +2715,7 @@
         <v>1</v>
       </c>
       <c r="AB16" t="s">
-        <v>237</v>
+        <v>235</v>
       </c>
     </row>
     <row r="17" spans="1:28">
@@ -2637,13 +2723,13 @@
         <v>24</v>
       </c>
       <c r="B17" t="s">
-        <v>229</v>
+        <v>227</v>
       </c>
       <c r="C17" t="s">
-        <v>207</v>
+        <v>205</v>
       </c>
       <c r="D17" t="s">
-        <v>208</v>
+        <v>206</v>
       </c>
       <c r="E17">
         <v>3</v>
@@ -2652,13 +2738,13 @@
         <v>2001</v>
       </c>
       <c r="G17" t="s">
-        <v>218</v>
+        <v>216</v>
       </c>
       <c r="H17">
         <v>1</v>
       </c>
       <c r="J17" t="s">
-        <v>212</v>
+        <v>210</v>
       </c>
       <c r="K17">
         <v>1</v>
@@ -2673,7 +2759,7 @@
         <v>30</v>
       </c>
       <c r="O17" t="s">
-        <v>210</v>
+        <v>208</v>
       </c>
       <c r="P17" t="s">
         <v>46</v>
@@ -2709,7 +2795,7 @@
         <v>1</v>
       </c>
       <c r="AB17" t="s">
-        <v>237</v>
+        <v>235</v>
       </c>
     </row>
     <row r="18" spans="1:28">
@@ -2717,13 +2803,13 @@
         <v>24</v>
       </c>
       <c r="B18" t="s">
-        <v>229</v>
+        <v>227</v>
       </c>
       <c r="C18" t="s">
-        <v>207</v>
+        <v>205</v>
       </c>
       <c r="D18" t="s">
-        <v>208</v>
+        <v>206</v>
       </c>
       <c r="E18">
         <v>3</v>
@@ -2756,7 +2842,7 @@
         <v>30</v>
       </c>
       <c r="O18" t="s">
-        <v>210</v>
+        <v>208</v>
       </c>
       <c r="P18" t="s">
         <v>46</v>
@@ -2792,7 +2878,7 @@
         <v>1</v>
       </c>
       <c r="AB18" t="s">
-        <v>237</v>
+        <v>235</v>
       </c>
     </row>
     <row r="19" spans="1:28">
@@ -2960,13 +3046,13 @@
         <v>24</v>
       </c>
       <c r="B21" t="s">
-        <v>230</v>
+        <v>228</v>
       </c>
       <c r="C21" t="s">
-        <v>199</v>
+        <v>197</v>
       </c>
       <c r="D21" t="s">
-        <v>200</v>
+        <v>198</v>
       </c>
       <c r="E21">
         <v>8</v>
@@ -2993,7 +3079,7 @@
         <v>2180</v>
       </c>
       <c r="O21" t="s">
-        <v>215</v>
+        <v>213</v>
       </c>
       <c r="P21" t="s">
         <v>46</v>
@@ -3032,7 +3118,7 @@
         <v>48</v>
       </c>
       <c r="AB21" t="s">
-        <v>231</v>
+        <v>229</v>
       </c>
     </row>
     <row r="22" spans="1:28">
@@ -3055,7 +3141,7 @@
         <v>1200</v>
       </c>
       <c r="G22" t="s">
-        <v>217</v>
+        <v>215</v>
       </c>
       <c r="H22">
         <v>1</v>
@@ -3378,7 +3464,7 @@
         <v>2002</v>
       </c>
       <c r="G26" t="s">
-        <v>216</v>
+        <v>214</v>
       </c>
       <c r="H26">
         <v>0</v>
@@ -3526,13 +3612,13 @@
         <v>24</v>
       </c>
       <c r="B28" t="s">
-        <v>232</v>
+        <v>230</v>
       </c>
       <c r="C28" t="s">
-        <v>219</v>
+        <v>217</v>
       </c>
       <c r="D28" t="s">
-        <v>220</v>
+        <v>218</v>
       </c>
       <c r="E28">
         <v>6</v>
@@ -3601,7 +3687,7 @@
         <v>105</v>
       </c>
       <c r="AB28" t="s">
-        <v>239</v>
+        <v>237</v>
       </c>
     </row>
     <row r="29" spans="1:28">
@@ -3609,13 +3695,13 @@
         <v>24</v>
       </c>
       <c r="B29" t="s">
-        <v>233</v>
+        <v>231</v>
       </c>
       <c r="C29" t="s">
-        <v>221</v>
+        <v>219</v>
       </c>
       <c r="D29" t="s">
-        <v>222</v>
+        <v>220</v>
       </c>
       <c r="E29">
         <v>6</v>
@@ -3645,7 +3731,7 @@
         <v>30</v>
       </c>
       <c r="O29" t="s">
-        <v>215</v>
+        <v>213</v>
       </c>
       <c r="P29" t="s">
         <v>46</v>
@@ -3684,7 +3770,7 @@
         <v>48</v>
       </c>
       <c r="AB29" t="s">
-        <v>241</v>
+        <v>239</v>
       </c>
     </row>
     <row r="30" spans="1:28">
@@ -3707,7 +3793,7 @@
         <v>1200</v>
       </c>
       <c r="G30" t="s">
-        <v>217</v>
+        <v>215</v>
       </c>
       <c r="H30">
         <v>1</v>
@@ -4012,13 +4098,13 @@
         <v>24</v>
       </c>
       <c r="B34" t="s">
-        <v>234</v>
+        <v>232</v>
       </c>
       <c r="C34" t="s">
-        <v>201</v>
+        <v>199</v>
       </c>
       <c r="D34" t="s">
-        <v>202</v>
+        <v>200</v>
       </c>
       <c r="E34">
         <v>8</v>
@@ -4084,7 +4170,7 @@
         <v>57</v>
       </c>
       <c r="AB34" t="s">
-        <v>235</v>
+        <v>233</v>
       </c>
     </row>
     <row r="35" spans="1:28">
@@ -4161,7 +4247,7 @@
         <v>1</v>
       </c>
       <c r="AB35" t="s">
-        <v>238</v>
+        <v>236</v>
       </c>
     </row>
   </sheetData>
@@ -4174,7 +4260,7 @@
   <dimension ref="A1:T10"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="T11" sqref="T11"/>
+      <selection activeCell="G3" sqref="G3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -4241,7 +4327,7 @@
         <v>60</v>
       </c>
       <c r="T1" s="12" t="s">
-        <v>246</v>
+        <v>244</v>
       </c>
     </row>
     <row r="2" spans="1:20" s="1" customFormat="1">
@@ -4261,7 +4347,7 @@
         <v>7731025.0201000012</v>
       </c>
       <c r="F2" s="4">
-        <v>69.35282494184429</v>
+        <v>69.352824941844304</v>
       </c>
       <c r="G2" s="4">
         <v>25.780663164598501</v>
@@ -4359,7 +4445,7 @@
         <v>0</v>
       </c>
       <c r="S3" s="1" t="s">
-        <v>150</v>
+        <v>148</v>
       </c>
       <c r="T3" s="4">
         <v>1</v>
@@ -4789,7 +4875,7 @@
   <dimension ref="A1:H34"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B30" sqref="B30"/>
+      <selection activeCell="A5" sqref="A5:E29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -4805,28 +4891,28 @@
   <sheetData>
     <row r="1" spans="1:8">
       <c r="A1" s="5" t="s">
+        <v>149</v>
+      </c>
+      <c r="B1" s="5" t="s">
+        <v>150</v>
+      </c>
+      <c r="C1" s="5" t="s">
         <v>151</v>
       </c>
-      <c r="B1" s="5" t="s">
+      <c r="D1" s="5" t="s">
         <v>152</v>
-      </c>
-      <c r="C1" s="5" t="s">
-        <v>153</v>
-      </c>
-      <c r="D1" s="5" t="s">
-        <v>154</v>
       </c>
       <c r="E1" s="5" t="s">
         <v>111</v>
       </c>
       <c r="F1" s="5" t="s">
-        <v>155</v>
+        <v>153</v>
       </c>
       <c r="G1" s="5" t="s">
-        <v>187</v>
+        <v>185</v>
       </c>
       <c r="H1" s="5" t="s">
-        <v>226</v>
+        <v>224</v>
       </c>
     </row>
     <row r="2" spans="1:8" hidden="1">
@@ -4834,7 +4920,7 @@
         <v>1</v>
       </c>
       <c r="B2" s="7" t="s">
-        <v>156</v>
+        <v>154</v>
       </c>
       <c r="C2" s="7">
         <v>68.8796064</v>
@@ -4844,7 +4930,7 @@
       </c>
       <c r="E2" s="7"/>
       <c r="F2" s="7" t="s">
-        <v>157</v>
+        <v>155</v>
       </c>
       <c r="G2" s="7">
         <v>0</v>
@@ -4855,7 +4941,7 @@
         <v>2</v>
       </c>
       <c r="B3" s="7" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
       <c r="C3" s="7">
         <v>69.016558200000006</v>
@@ -4865,7 +4951,7 @@
       </c>
       <c r="E3" s="7"/>
       <c r="F3" s="7" t="s">
-        <v>157</v>
+        <v>155</v>
       </c>
       <c r="G3" s="7">
         <v>0</v>
@@ -4876,7 +4962,7 @@
         <v>3</v>
       </c>
       <c r="B4" s="7" t="s">
-        <v>159</v>
+        <v>157</v>
       </c>
       <c r="C4" s="7">
         <v>69.091232599999998</v>
@@ -4886,7 +4972,7 @@
       </c>
       <c r="E4" s="7"/>
       <c r="F4" s="7" t="s">
-        <v>157</v>
+        <v>155</v>
       </c>
       <c r="G4" s="7">
         <v>0</v>
@@ -4897,7 +4983,7 @@
         <v>4</v>
       </c>
       <c r="B5" s="7" t="s">
-        <v>160</v>
+        <v>158</v>
       </c>
       <c r="C5" s="7">
         <v>68.926158000000001</v>
@@ -4906,10 +4992,10 @@
         <v>25.597493</v>
       </c>
       <c r="E5" s="7" t="s">
-        <v>252</v>
+        <v>250</v>
       </c>
       <c r="F5" s="7" t="s">
-        <v>192</v>
+        <v>190</v>
       </c>
       <c r="G5" s="7">
         <v>1</v>
@@ -4923,7 +5009,7 @@
         <v>6</v>
       </c>
       <c r="B6" s="7" t="s">
-        <v>161</v>
+        <v>159</v>
       </c>
       <c r="C6" s="7">
         <v>69.594406199999995</v>
@@ -4933,7 +5019,7 @@
       </c>
       <c r="E6" s="7"/>
       <c r="F6" s="7" t="s">
-        <v>157</v>
+        <v>155</v>
       </c>
       <c r="G6" s="7">
         <v>0</v>
@@ -4944,7 +5030,7 @@
         <v>7</v>
       </c>
       <c r="B7" s="7" t="s">
-        <v>162</v>
+        <v>160</v>
       </c>
       <c r="C7" s="7">
         <v>69.876856700000005</v>
@@ -4954,7 +5040,7 @@
       </c>
       <c r="E7" s="7"/>
       <c r="F7" s="7" t="s">
-        <v>157</v>
+        <v>155</v>
       </c>
       <c r="G7" s="7">
         <v>0</v>
@@ -4965,7 +5051,7 @@
         <v>8</v>
       </c>
       <c r="B8" s="7" t="s">
-        <v>163</v>
+        <v>161</v>
       </c>
       <c r="C8" s="7">
         <v>69.958485800000005</v>
@@ -4974,10 +5060,10 @@
         <v>26.862095</v>
       </c>
       <c r="E8" s="7" t="s">
-        <v>252</v>
+        <v>250</v>
       </c>
       <c r="F8" s="7" t="s">
-        <v>193</v>
+        <v>191</v>
       </c>
       <c r="G8" s="7">
         <v>1</v>
@@ -4991,7 +5077,7 @@
         <v>9</v>
       </c>
       <c r="B9" s="7" t="s">
-        <v>164</v>
+        <v>162</v>
       </c>
       <c r="C9" s="7">
         <v>69.965898899999999</v>
@@ -5001,7 +5087,7 @@
       </c>
       <c r="E9" s="7"/>
       <c r="F9" s="7" t="s">
-        <v>157</v>
+        <v>155</v>
       </c>
       <c r="G9" s="7">
         <v>0</v>
@@ -5012,7 +5098,7 @@
         <v>10</v>
       </c>
       <c r="B10" s="7" t="s">
-        <v>165</v>
+        <v>163</v>
       </c>
       <c r="C10" s="7">
         <v>70.127020200000004</v>
@@ -5022,7 +5108,7 @@
       </c>
       <c r="E10" s="7"/>
       <c r="F10" s="7" t="s">
-        <v>157</v>
+        <v>155</v>
       </c>
       <c r="G10" s="7">
         <v>0</v>
@@ -5033,7 +5119,7 @@
         <v>11</v>
       </c>
       <c r="B11" s="7" t="s">
-        <v>166</v>
+        <v>164</v>
       </c>
       <c r="C11" s="7">
         <v>68.869617700000006</v>
@@ -5043,7 +5129,7 @@
       </c>
       <c r="E11" s="7"/>
       <c r="F11" s="7" t="s">
-        <v>167</v>
+        <v>165</v>
       </c>
       <c r="G11" s="7">
         <v>0</v>
@@ -5054,7 +5140,7 @@
         <v>12</v>
       </c>
       <c r="B12" s="7" t="s">
-        <v>168</v>
+        <v>166</v>
       </c>
       <c r="C12" s="7">
         <v>69.338290299999997</v>
@@ -5063,10 +5149,10 @@
         <v>25.098504399999999</v>
       </c>
       <c r="E12" s="7" t="s">
-        <v>252</v>
+        <v>250</v>
       </c>
       <c r="F12" s="7" t="s">
-        <v>190</v>
+        <v>188</v>
       </c>
       <c r="G12" s="7">
         <v>1</v>
@@ -5080,7 +5166,7 @@
         <v>13</v>
       </c>
       <c r="B13" s="7" t="s">
-        <v>169</v>
+        <v>167</v>
       </c>
       <c r="C13" s="7">
         <v>69.106753400000002</v>
@@ -5089,10 +5175,10 @@
         <v>25.7197402</v>
       </c>
       <c r="E13" s="7" t="s">
-        <v>252</v>
+        <v>250</v>
       </c>
       <c r="F13" s="7" t="s">
-        <v>194</v>
+        <v>192</v>
       </c>
       <c r="G13" s="7">
         <v>1</v>
@@ -5106,7 +5192,7 @@
         <v>14</v>
       </c>
       <c r="B14" s="7" t="s">
-        <v>172</v>
+        <v>170</v>
       </c>
       <c r="C14" s="7">
         <v>69.38992184</v>
@@ -5115,7 +5201,7 @@
         <v>24.472635199999999</v>
       </c>
       <c r="E14" s="7" t="s">
-        <v>252</v>
+        <v>250</v>
       </c>
       <c r="F14" s="7" t="s">
         <v>146</v>
@@ -5129,10 +5215,10 @@
     </row>
     <row r="15" spans="1:8" hidden="1">
       <c r="A15" s="6" t="s">
-        <v>185</v>
+        <v>183</v>
       </c>
       <c r="B15" s="7" t="s">
-        <v>186</v>
+        <v>184</v>
       </c>
       <c r="C15" s="7">
         <v>70.29406007</v>
@@ -5142,7 +5228,7 @@
       </c>
       <c r="E15" s="7"/>
       <c r="F15" s="7" t="s">
-        <v>157</v>
+        <v>155</v>
       </c>
       <c r="G15" s="7">
         <v>0</v>
@@ -5150,10 +5236,10 @@
     </row>
     <row r="16" spans="1:8">
       <c r="A16" s="6" t="s">
-        <v>170</v>
+        <v>168</v>
       </c>
       <c r="B16" s="7" t="s">
-        <v>171</v>
+        <v>169</v>
       </c>
       <c r="C16" s="7">
         <v>69.199913890000005</v>
@@ -5162,10 +5248,10 @@
         <v>25.689412659999999</v>
       </c>
       <c r="E16" s="7" t="s">
-        <v>252</v>
+        <v>250</v>
       </c>
       <c r="F16" s="7" t="s">
-        <v>195</v>
+        <v>193</v>
       </c>
       <c r="G16" s="7">
         <v>1</v>
@@ -5176,10 +5262,10 @@
     </row>
     <row r="17" spans="1:8" hidden="1">
       <c r="A17" s="6" t="s">
-        <v>173</v>
+        <v>171</v>
       </c>
       <c r="B17" s="7" t="s">
-        <v>174</v>
+        <v>172</v>
       </c>
       <c r="C17" s="7">
         <v>68.994171269999995</v>
@@ -5189,7 +5275,7 @@
       </c>
       <c r="E17" s="7"/>
       <c r="F17" s="7" t="s">
-        <v>157</v>
+        <v>155</v>
       </c>
       <c r="G17" s="7">
         <v>0</v>
@@ -5197,10 +5283,10 @@
     </row>
     <row r="18" spans="1:8" hidden="1">
       <c r="A18" s="6" t="s">
-        <v>175</v>
+        <v>173</v>
       </c>
       <c r="B18" s="7" t="s">
-        <v>176</v>
+        <v>174</v>
       </c>
       <c r="C18" s="7">
         <v>69.33199879</v>
@@ -5210,7 +5296,7 @@
       </c>
       <c r="E18" s="7"/>
       <c r="F18" s="7" t="s">
-        <v>157</v>
+        <v>155</v>
       </c>
       <c r="G18" s="7">
         <v>0</v>
@@ -5218,10 +5304,10 @@
     </row>
     <row r="19" spans="1:8">
       <c r="A19" s="6" t="s">
-        <v>177</v>
+        <v>175</v>
       </c>
       <c r="B19" s="7" t="s">
-        <v>178</v>
+        <v>176</v>
       </c>
       <c r="C19" s="7">
         <v>69.327241860000001</v>
@@ -5230,10 +5316,10 @@
         <v>24.010010829999999</v>
       </c>
       <c r="E19" s="7" t="s">
-        <v>252</v>
+        <v>250</v>
       </c>
       <c r="F19" s="7" t="s">
-        <v>196</v>
+        <v>194</v>
       </c>
       <c r="G19" s="7">
         <v>1</v>
@@ -5244,10 +5330,10 @@
     </row>
     <row r="20" spans="1:8">
       <c r="A20" s="6" t="s">
-        <v>179</v>
+        <v>177</v>
       </c>
       <c r="B20" s="7" t="s">
-        <v>180</v>
+        <v>178</v>
       </c>
       <c r="C20" s="7">
         <v>69.534884730000002</v>
@@ -5256,10 +5342,10 @@
         <v>24.890296469999999</v>
       </c>
       <c r="E20" s="7" t="s">
-        <v>252</v>
+        <v>250</v>
       </c>
       <c r="F20" s="7" t="s">
-        <v>197</v>
+        <v>195</v>
       </c>
       <c r="G20" s="7">
         <v>1</v>
@@ -5270,10 +5356,10 @@
     </row>
     <row r="21" spans="1:8" hidden="1">
       <c r="A21" s="6" t="s">
-        <v>181</v>
+        <v>179</v>
       </c>
       <c r="B21" s="7" t="s">
-        <v>182</v>
+        <v>180</v>
       </c>
       <c r="C21" s="7">
         <v>69.960127920000005</v>
@@ -5283,7 +5369,7 @@
       </c>
       <c r="E21" s="7"/>
       <c r="F21" s="7" t="s">
-        <v>189</v>
+        <v>187</v>
       </c>
       <c r="G21" s="7">
         <v>0</v>
@@ -5291,10 +5377,10 @@
     </row>
     <row r="22" spans="1:8">
       <c r="A22" s="6" t="s">
-        <v>183</v>
+        <v>181</v>
       </c>
       <c r="B22" s="7" t="s">
-        <v>184</v>
+        <v>182</v>
       </c>
       <c r="C22" s="7">
         <v>69.967677710000004</v>
@@ -5303,10 +5389,10 @@
         <v>26.424932210000001</v>
       </c>
       <c r="E22" s="7" t="s">
-        <v>252</v>
+        <v>250</v>
       </c>
       <c r="F22" s="7" t="s">
-        <v>191</v>
+        <v>189</v>
       </c>
       <c r="G22" s="7">
         <v>1</v>
@@ -5317,10 +5403,10 @@
     </row>
     <row r="23" spans="1:8">
       <c r="A23" s="16" t="s">
-        <v>261</v>
+        <v>259</v>
       </c>
       <c r="B23" s="16" t="s">
-        <v>258</v>
+        <v>256</v>
       </c>
       <c r="C23" s="7">
         <v>69.445760000000007</v>
@@ -5329,7 +5415,7 @@
         <v>25.355440000000002</v>
       </c>
       <c r="E23" s="7" t="s">
-        <v>253</v>
+        <v>251</v>
       </c>
       <c r="G23" s="7">
         <v>1</v>
@@ -5340,10 +5426,10 @@
     </row>
     <row r="24" spans="1:8">
       <c r="A24" s="17" t="s">
-        <v>257</v>
+        <v>255</v>
       </c>
       <c r="B24" s="19" t="s">
-        <v>262</v>
+        <v>260</v>
       </c>
       <c r="C24" s="7">
         <v>69.426199999999994</v>
@@ -5352,7 +5438,7 @@
         <v>24.940829999999998</v>
       </c>
       <c r="E24" s="7" t="s">
-        <v>253</v>
+        <v>251</v>
       </c>
       <c r="G24" s="7">
         <v>1</v>
@@ -5363,10 +5449,10 @@
     </row>
     <row r="25" spans="1:8">
       <c r="A25" s="17" t="s">
-        <v>260</v>
+        <v>258</v>
       </c>
       <c r="B25" s="7" t="s">
-        <v>255</v>
+        <v>253</v>
       </c>
       <c r="C25" s="7">
         <v>69.419210000000007</v>
@@ -5375,7 +5461,7 @@
         <v>25.159690000000001</v>
       </c>
       <c r="E25" s="7" t="s">
-        <v>253</v>
+        <v>251</v>
       </c>
       <c r="G25" s="7">
         <v>1</v>
@@ -5386,10 +5472,10 @@
     </row>
     <row r="26" spans="1:8">
       <c r="A26" s="18" t="s">
-        <v>259</v>
+        <v>257</v>
       </c>
       <c r="B26" s="7" t="s">
-        <v>263</v>
+        <v>261</v>
       </c>
       <c r="C26" s="7">
         <v>69.468090000000004</v>
@@ -5398,7 +5484,7 @@
         <v>25.507429999999999</v>
       </c>
       <c r="E26" s="7" t="s">
-        <v>253</v>
+        <v>251</v>
       </c>
       <c r="G26" s="7">
         <v>1</v>
@@ -5409,10 +5495,10 @@
     </row>
     <row r="27" spans="1:8">
       <c r="A27" s="17" t="s">
-        <v>256</v>
+        <v>254</v>
       </c>
       <c r="B27" s="17" t="s">
-        <v>249</v>
+        <v>247</v>
       </c>
       <c r="C27" s="7">
         <v>69.39837</v>
@@ -5421,7 +5507,7 @@
         <v>25.842220000000001</v>
       </c>
       <c r="E27" s="7" t="s">
-        <v>253</v>
+        <v>251</v>
       </c>
       <c r="G27" s="7">
         <v>1</v>
@@ -5432,10 +5518,10 @@
     </row>
     <row r="28" spans="1:8">
       <c r="A28" s="16" t="s">
-        <v>188</v>
+        <v>186</v>
       </c>
       <c r="B28" s="16" t="s">
-        <v>188</v>
+        <v>186</v>
       </c>
       <c r="C28" s="7">
         <v>69.908649999999994</v>
@@ -5444,7 +5530,7 @@
         <v>27.047160000000002</v>
       </c>
       <c r="E28" s="7" t="s">
-        <v>253</v>
+        <v>251</v>
       </c>
       <c r="G28" s="7">
         <v>1</v>
@@ -5455,10 +5541,10 @@
     </row>
     <row r="29" spans="1:8" ht="15.75" customHeight="1">
       <c r="A29" s="16" t="s">
-        <v>254</v>
+        <v>252</v>
       </c>
       <c r="B29" s="16" t="s">
-        <v>264</v>
+        <v>262</v>
       </c>
       <c r="C29" s="7">
         <v>70.074259999999995</v>
@@ -5467,7 +5553,7 @@
         <v>28.057860000000002</v>
       </c>
       <c r="E29" s="7" t="s">
-        <v>253</v>
+        <v>251</v>
       </c>
       <c r="G29" s="7">
         <v>1</v>
@@ -5519,10 +5605,10 @@
   <sheetData>
     <row r="1" spans="1:4">
       <c r="A1" t="s">
-        <v>151</v>
+        <v>149</v>
       </c>
       <c r="B1" t="s">
-        <v>152</v>
+        <v>150</v>
       </c>
       <c r="C1" t="s">
         <v>114</v>
@@ -5533,7 +5619,7 @@
     </row>
     <row r="2" spans="1:4">
       <c r="A2" t="s">
-        <v>247</v>
+        <v>245</v>
       </c>
       <c r="B2" t="s">
         <v>49</v>
@@ -5547,10 +5633,10 @@
     </row>
     <row r="3" spans="1:4">
       <c r="A3" t="s">
-        <v>248</v>
+        <v>246</v>
       </c>
       <c r="B3" s="14" t="s">
-        <v>249</v>
+        <v>247</v>
       </c>
       <c r="C3" s="15">
         <v>69.398449999999997</v>
@@ -5561,10 +5647,10 @@
     </row>
     <row r="4" spans="1:4">
       <c r="A4" t="s">
-        <v>250</v>
+        <v>248</v>
       </c>
       <c r="B4" s="14" t="s">
-        <v>251</v>
+        <v>249</v>
       </c>
       <c r="C4" s="15">
         <v>69.397360000000006</v>
@@ -5575,10 +5661,10 @@
     </row>
     <row r="5" spans="1:4">
       <c r="A5" s="6" t="s">
-        <v>177</v>
+        <v>175</v>
       </c>
       <c r="B5" s="7" t="s">
-        <v>178</v>
+        <v>176</v>
       </c>
       <c r="C5" s="7">
         <v>69.327241860000001</v>
@@ -5589,10 +5675,10 @@
     </row>
     <row r="6" spans="1:4">
       <c r="A6" s="6" t="s">
-        <v>183</v>
+        <v>181</v>
       </c>
       <c r="B6" s="7" t="s">
-        <v>184</v>
+        <v>182</v>
       </c>
       <c r="C6" s="7">
         <v>69.967677710000004</v>
@@ -5603,10 +5689,10 @@
     </row>
     <row r="7" spans="1:4">
       <c r="A7" s="6" t="s">
-        <v>170</v>
+        <v>168</v>
       </c>
       <c r="B7" s="7" t="s">
-        <v>171</v>
+        <v>169</v>
       </c>
       <c r="C7" s="7">
         <v>69.199913890000005</v>
@@ -5639,7 +5725,7 @@
   <dimension ref="A1:G3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="N35" sqref="N35"/>
+      <selection activeCell="A2" sqref="A2:D3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -5649,19 +5735,19 @@
   <sheetData>
     <row r="1" spans="1:7">
       <c r="A1" s="5" t="s">
+        <v>149</v>
+      </c>
+      <c r="B1" s="5" t="s">
+        <v>150</v>
+      </c>
+      <c r="C1" s="5" t="s">
         <v>151</v>
       </c>
-      <c r="B1" s="5" t="s">
+      <c r="D1" s="5" t="s">
         <v>152</v>
       </c>
-      <c r="C1" s="5" t="s">
-        <v>153</v>
-      </c>
-      <c r="D1" s="5" t="s">
-        <v>154</v>
-      </c>
       <c r="E1" t="s">
-        <v>242</v>
+        <v>240</v>
       </c>
       <c r="F1" t="s">
         <v>60</v>
@@ -5669,10 +5755,10 @@
     </row>
     <row r="2" spans="1:7">
       <c r="A2" t="s">
-        <v>243</v>
+        <v>241</v>
       </c>
       <c r="B2" t="s">
-        <v>243</v>
+        <v>241</v>
       </c>
       <c r="C2">
         <v>70.023740000000004</v>
@@ -5681,21 +5767,21 @@
         <v>28.04233</v>
       </c>
       <c r="E2" t="s">
-        <v>244</v>
+        <v>242</v>
       </c>
       <c r="F2" t="s">
-        <v>245</v>
+        <v>243</v>
       </c>
     </row>
     <row r="3" spans="1:7">
       <c r="A3" s="6" t="s">
-        <v>224</v>
+        <v>222</v>
       </c>
       <c r="B3" t="s">
-        <v>225</v>
+        <v>223</v>
       </c>
       <c r="C3" t="s">
-        <v>223</v>
+        <v>221</v>
       </c>
       <c r="D3">
         <v>25.39873</v>
@@ -5709,756 +5795,1808 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B293E105-2DEC-4AB0-8F8B-0F0216933BBC}">
-  <dimension ref="A1:G32"/>
+  <dimension ref="A1:F36"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J22" sqref="J22"/>
+      <selection activeCell="D21" sqref="D21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="2" max="2" width="34.42578125" bestFit="1" customWidth="1"/>
+    <col min="3" max="4" width="9.140625" style="24"/>
+    <col min="5" max="5" width="19.42578125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="79.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" s="1" customFormat="1">
-      <c r="A1" s="1" t="s">
+    <row r="1" spans="1:6" s="20" customFormat="1">
+      <c r="A1" s="20" t="s">
         <v>2</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="B1" s="20" t="s">
         <v>3</v>
       </c>
-      <c r="C1" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="E1" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="F1" s="1" t="s">
+      <c r="C1" s="21" t="s">
+        <v>264</v>
+      </c>
+      <c r="D1" s="21" t="s">
+        <v>263</v>
+      </c>
+      <c r="E1" s="20" t="s">
         <v>111</v>
       </c>
-      <c r="G1" s="1" t="s">
-        <v>149</v>
-      </c>
-    </row>
-    <row r="2" spans="1:7" s="1" customFormat="1">
-      <c r="A2" s="1" t="s">
-        <v>57</v>
-      </c>
-      <c r="B2" s="1" t="s">
-        <v>58</v>
-      </c>
-      <c r="C2" s="1" t="s">
-        <v>34</v>
-      </c>
-      <c r="D2" s="1">
-        <v>24.938338000000002</v>
-      </c>
-      <c r="E2" s="1">
-        <v>69.426393000000004</v>
-      </c>
-      <c r="F2" s="1" t="s">
+      <c r="F1" s="20" t="s">
+        <v>265</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" s="1" customFormat="1">
+      <c r="A2" s="6">
+        <v>4</v>
+      </c>
+      <c r="B2" s="7" t="s">
+        <v>158</v>
+      </c>
+      <c r="C2" s="22">
+        <v>68.926158000000001</v>
+      </c>
+      <c r="D2" s="22">
+        <v>25.597493</v>
+      </c>
+      <c r="E2" s="7" t="s">
+        <v>196</v>
+      </c>
+      <c r="F2" s="7" t="s">
+        <v>275</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" s="1" customFormat="1">
+      <c r="A3" s="6">
+        <v>13</v>
+      </c>
+      <c r="B3" s="7" t="s">
+        <v>167</v>
+      </c>
+      <c r="C3" s="22">
+        <v>69.106753400000002</v>
+      </c>
+      <c r="D3" s="22">
+        <v>25.7197402</v>
+      </c>
+      <c r="E3" s="7" t="s">
+        <v>196</v>
+      </c>
+      <c r="F3" s="7" t="s">
+        <v>275</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" s="1" customFormat="1">
+      <c r="A4" s="6" t="s">
+        <v>168</v>
+      </c>
+      <c r="B4" s="7" t="s">
+        <v>169</v>
+      </c>
+      <c r="C4" s="22">
+        <v>69.199913890000005</v>
+      </c>
+      <c r="D4" s="22">
+        <v>25.689412659999999</v>
+      </c>
+      <c r="E4" s="7" t="s">
+        <v>196</v>
+      </c>
+      <c r="F4" s="7" t="s">
+        <v>276</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" s="1" customFormat="1">
+      <c r="A5" s="6" t="s">
+        <v>175</v>
+      </c>
+      <c r="B5" s="7" t="s">
+        <v>176</v>
+      </c>
+      <c r="C5" s="22">
+        <v>69.327241860000001</v>
+      </c>
+      <c r="D5" s="22">
+        <v>24.010010829999999</v>
+      </c>
+      <c r="E5" s="7" t="s">
+        <v>196</v>
+      </c>
+      <c r="F5" s="7" t="s">
+        <v>276</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" s="1" customFormat="1">
+      <c r="A6" s="6">
+        <v>12</v>
+      </c>
+      <c r="B6" s="7" t="s">
+        <v>166</v>
+      </c>
+      <c r="C6" s="22">
+        <v>69.338290299999997</v>
+      </c>
+      <c r="D6" s="22">
+        <v>25.098504399999999</v>
+      </c>
+      <c r="E6" s="7" t="s">
+        <v>196</v>
+      </c>
+      <c r="F6" s="7" t="s">
+        <v>275</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" s="1" customFormat="1">
+      <c r="A7" s="4" t="s">
+        <v>127</v>
+      </c>
+      <c r="B7" s="4" t="s">
+        <v>128</v>
+      </c>
+      <c r="C7" s="23">
+        <v>69.352824941844304</v>
+      </c>
+      <c r="D7" s="23">
+        <v>25.780663164598501</v>
+      </c>
+      <c r="E7" s="4" t="s">
+        <v>147</v>
+      </c>
+      <c r="F7" s="4" t="s">
+        <v>274</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" s="1" customFormat="1">
+      <c r="A8" s="6">
+        <v>14</v>
+      </c>
+      <c r="B8" s="7" t="s">
+        <v>170</v>
+      </c>
+      <c r="C8" s="22">
+        <v>69.38992184</v>
+      </c>
+      <c r="D8" s="22">
+        <v>24.472635199999999</v>
+      </c>
+      <c r="E8" s="7" t="s">
+        <v>277</v>
+      </c>
+      <c r="F8" s="7" t="s">
+        <v>278</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" s="1" customFormat="1">
+      <c r="A9" s="17" t="s">
+        <v>254</v>
+      </c>
+      <c r="B9" s="17" t="s">
+        <v>247</v>
+      </c>
+      <c r="C9" s="22">
+        <v>69.39837</v>
+      </c>
+      <c r="D9" s="22">
+        <v>25.842220000000001</v>
+      </c>
+      <c r="E9" s="7" t="s">
+        <v>196</v>
+      </c>
+      <c r="F9" s="7" t="s">
+        <v>276</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" s="1" customFormat="1">
+      <c r="A10" t="s">
+        <v>205</v>
+      </c>
+      <c r="B10" t="s">
+        <v>206</v>
+      </c>
+      <c r="C10" s="24">
+        <v>69.400858999999997</v>
+      </c>
+      <c r="D10" s="24">
+        <v>25.814402000000001</v>
+      </c>
+      <c r="E10" s="7" t="s">
         <v>146</v>
       </c>
-      <c r="G2" s="1">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="3" spans="1:7" s="1" customFormat="1">
-      <c r="A3" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="B3" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="C3" s="1" t="s">
-        <v>34</v>
-      </c>
-      <c r="D3" s="1">
-        <v>24.474238</v>
-      </c>
-      <c r="E3" s="1">
-        <v>69.390030999999993</v>
-      </c>
-      <c r="F3" s="1" t="s">
+      <c r="F10" t="s">
+        <v>269</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" s="1" customFormat="1">
+      <c r="A11" s="1" t="s">
+        <v>73</v>
+      </c>
+      <c r="B11" s="1" t="s">
+        <v>74</v>
+      </c>
+      <c r="C11" s="23">
+        <v>69.408237</v>
+      </c>
+      <c r="D11" s="23">
+        <v>25.811848999999999</v>
+      </c>
+      <c r="E11" s="1" t="s">
         <v>146</v>
       </c>
-      <c r="G3" s="1">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="4" spans="1:7" s="1" customFormat="1">
-      <c r="A4" s="1" t="s">
-        <v>42</v>
-      </c>
-      <c r="B4" s="1" t="s">
-        <v>43</v>
-      </c>
-      <c r="C4" s="1" t="s">
-        <v>34</v>
-      </c>
-      <c r="D4" s="1">
-        <v>25.158322999999999</v>
-      </c>
-      <c r="E4" s="1">
-        <v>69.419317000000007</v>
-      </c>
-      <c r="F4" s="1" t="s">
-        <v>146</v>
-      </c>
-      <c r="G4" s="1">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="5" spans="1:7" s="1" customFormat="1">
-      <c r="A5" s="1" t="s">
-        <v>36</v>
-      </c>
-      <c r="B5" s="1" t="s">
-        <v>37</v>
-      </c>
-      <c r="C5" s="1" t="s">
-        <v>34</v>
-      </c>
-      <c r="D5" s="1">
-        <v>24.388183000000001</v>
-      </c>
-      <c r="E5" s="1">
-        <v>69.565611000000004</v>
-      </c>
-      <c r="F5" s="1" t="s">
-        <v>146</v>
-      </c>
-      <c r="G5" s="1">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="6" spans="1:7" s="1" customFormat="1">
-      <c r="A6" s="1" t="s">
-        <v>52</v>
-      </c>
-      <c r="B6" s="1" t="s">
-        <v>53</v>
-      </c>
-      <c r="C6" s="1" t="s">
-        <v>34</v>
-      </c>
-      <c r="D6" s="1">
-        <v>28.041376</v>
-      </c>
-      <c r="E6" s="1">
-        <v>70.419150999999999</v>
-      </c>
-      <c r="F6" s="1" t="s">
-        <v>146</v>
-      </c>
-      <c r="G6" s="1">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="7" spans="1:7" s="1" customFormat="1">
-      <c r="A7" s="1" t="s">
-        <v>66</v>
-      </c>
-      <c r="B7" s="1" t="s">
-        <v>67</v>
-      </c>
-      <c r="C7" s="1" t="s">
-        <v>34</v>
-      </c>
-      <c r="D7" s="1">
-        <v>25.510739000000001</v>
-      </c>
-      <c r="E7" s="1">
-        <v>69.469237000000007</v>
-      </c>
-      <c r="F7" s="1" t="s">
-        <v>146</v>
-      </c>
-      <c r="G7" s="1">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="8" spans="1:7" s="1" customFormat="1">
-      <c r="A8" s="2" t="s">
-        <v>99</v>
-      </c>
-      <c r="B8" s="2" t="s">
-        <v>100</v>
-      </c>
-      <c r="C8" s="2" t="s">
-        <v>34</v>
-      </c>
-      <c r="D8" s="2">
-        <v>28.824532000000001</v>
-      </c>
-      <c r="E8" s="2">
-        <v>70.472215000000006</v>
-      </c>
-      <c r="F8" s="1" t="s">
-        <v>146</v>
-      </c>
-      <c r="G8" s="2">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="9" spans="1:7" s="1" customFormat="1">
-      <c r="A9" s="1" t="s">
-        <v>48</v>
-      </c>
-      <c r="B9" s="1" t="s">
-        <v>49</v>
-      </c>
-      <c r="C9" s="1" t="s">
-        <v>34</v>
-      </c>
-      <c r="D9" s="1">
-        <v>28.016017000000002</v>
-      </c>
-      <c r="E9" s="1">
-        <v>70.070346999999998</v>
-      </c>
-      <c r="F9" s="1" t="s">
-        <v>146</v>
-      </c>
-      <c r="G9" s="1">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="10" spans="1:7" s="1" customFormat="1">
-      <c r="A10" s="1" t="s">
-        <v>73</v>
-      </c>
-      <c r="B10" s="1" t="s">
-        <v>74</v>
-      </c>
-      <c r="C10" s="1" t="s">
-        <v>34</v>
-      </c>
-      <c r="D10" s="1">
-        <v>25.811848999999999</v>
-      </c>
-      <c r="E10" s="1">
-        <v>69.408237</v>
-      </c>
-      <c r="F10" s="1" t="s">
-        <v>146</v>
-      </c>
-      <c r="G10" s="1">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="11" spans="1:7" s="1" customFormat="1">
-      <c r="A11" s="1" t="s">
-        <v>78</v>
-      </c>
-      <c r="B11" s="1" t="s">
-        <v>79</v>
-      </c>
-      <c r="C11" s="1" t="s">
-        <v>34</v>
-      </c>
-      <c r="D11" s="1">
-        <v>26.485793000000001</v>
-      </c>
-      <c r="E11" s="1">
-        <v>69.944618000000006</v>
-      </c>
       <c r="F11" s="1" t="s">
-        <v>146</v>
-      </c>
-      <c r="G11" s="1">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="12" spans="1:7" s="1" customFormat="1">
-      <c r="A12" s="1" t="s">
-        <v>84</v>
-      </c>
-      <c r="B12" s="1" t="s">
-        <v>85</v>
-      </c>
-      <c r="C12" s="1" t="s">
-        <v>34</v>
-      </c>
-      <c r="D12" s="1">
-        <v>28.22343</v>
-      </c>
-      <c r="E12" s="1">
-        <v>70.166214999999994</v>
-      </c>
-      <c r="F12" s="1" t="s">
-        <v>146</v>
-      </c>
-      <c r="G12" s="1">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="13" spans="1:7" s="1" customFormat="1">
-      <c r="A13" s="1" t="s">
-        <v>91</v>
-      </c>
-      <c r="B13" s="1" t="s">
-        <v>92</v>
-      </c>
-      <c r="C13" s="1" t="s">
-        <v>34</v>
-      </c>
-      <c r="D13" s="1">
-        <v>28.249378</v>
-      </c>
-      <c r="E13" s="1">
-        <v>70.375489999999999</v>
-      </c>
-      <c r="F13" s="1" t="s">
-        <v>146</v>
-      </c>
-      <c r="G13" s="1">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="14" spans="1:7" s="1" customFormat="1">
-      <c r="A14" s="1" t="s">
-        <v>105</v>
-      </c>
-      <c r="B14" s="1" t="s">
-        <v>106</v>
-      </c>
-      <c r="C14" s="1" t="s">
-        <v>34</v>
-      </c>
-      <c r="D14" s="1">
-        <v>27.705573000000001</v>
-      </c>
-      <c r="E14" s="1">
-        <v>70.074292</v>
-      </c>
-      <c r="F14" s="1" t="s">
-        <v>146</v>
-      </c>
-      <c r="G14" s="1">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="15" spans="1:7">
+        <v>273</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" s="1" customFormat="1">
+      <c r="A12" s="17" t="s">
+        <v>258</v>
+      </c>
+      <c r="B12" s="7" t="s">
+        <v>253</v>
+      </c>
+      <c r="C12" s="22">
+        <v>69.419210000000007</v>
+      </c>
+      <c r="D12" s="22">
+        <v>25.159690000000001</v>
+      </c>
+      <c r="E12" s="7" t="s">
+        <v>277</v>
+      </c>
+      <c r="F12" s="7" t="s">
+        <v>279</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" s="1" customFormat="1">
+      <c r="A13" s="17" t="s">
+        <v>281</v>
+      </c>
+      <c r="B13" s="18" t="s">
+        <v>260</v>
+      </c>
+      <c r="C13" s="22">
+        <v>69.426199999999994</v>
+      </c>
+      <c r="D13" s="22">
+        <v>24.940829999999998</v>
+      </c>
+      <c r="E13" s="7" t="s">
+        <v>277</v>
+      </c>
+      <c r="F13" s="7" t="s">
+        <v>280</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6">
+      <c r="A14" s="6" t="s">
+        <v>222</v>
+      </c>
+      <c r="B14" t="s">
+        <v>223</v>
+      </c>
+      <c r="C14" s="24">
+        <v>69.439130000000006</v>
+      </c>
+      <c r="D14" s="24">
+        <v>25.39873</v>
+      </c>
+      <c r="E14" s="7" t="s">
+        <v>222</v>
+      </c>
+      <c r="F14" s="7" t="s">
+        <v>270</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6">
       <c r="A15" s="4" t="s">
-        <v>127</v>
+        <v>132</v>
       </c>
       <c r="B15" s="4" t="s">
-        <v>128</v>
-      </c>
-      <c r="C15" s="4" t="s">
+        <v>133</v>
+      </c>
+      <c r="C15" s="23">
+        <v>69.442455747083997</v>
+      </c>
+      <c r="D15" s="23">
+        <v>25.691932628253909</v>
+      </c>
+      <c r="E15" s="4" t="s">
         <v>147</v>
       </c>
-      <c r="D15" s="4">
-        <v>25.780663164598501</v>
-      </c>
-      <c r="E15" s="4">
-        <v>69.35282494184429</v>
-      </c>
       <c r="F15" s="4" t="s">
-        <v>148</v>
-      </c>
-      <c r="G15" s="1">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="16" spans="1:7">
+        <v>274</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6">
       <c r="A16" s="4" t="s">
         <v>130</v>
       </c>
       <c r="B16" s="4" t="s">
         <v>131</v>
       </c>
-      <c r="C16" s="4" t="s">
+      <c r="C16" s="23">
+        <v>69.443804309461029</v>
+      </c>
+      <c r="D16" s="23">
+        <v>25.21361834597635</v>
+      </c>
+      <c r="E16" s="4" t="s">
         <v>147</v>
       </c>
-      <c r="D16" s="4">
-        <v>25.21361834597635</v>
-      </c>
-      <c r="E16" s="4">
-        <v>69.443804309461029</v>
-      </c>
       <c r="F16" s="4" t="s">
-        <v>148</v>
-      </c>
-      <c r="G16" s="1">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="17" spans="1:7">
-      <c r="A17" s="4" t="s">
-        <v>132</v>
-      </c>
-      <c r="B17" s="4" t="s">
-        <v>133</v>
-      </c>
-      <c r="C17" s="4" t="s">
-        <v>147</v>
-      </c>
-      <c r="D17" s="4">
-        <v>25.691932628253909</v>
-      </c>
-      <c r="E17" s="4">
-        <v>69.442455747083997</v>
-      </c>
-      <c r="F17" s="4" t="s">
-        <v>148</v>
-      </c>
-      <c r="G17" s="1">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="18" spans="1:7">
-      <c r="A18" s="4" t="s">
-        <v>134</v>
-      </c>
-      <c r="B18" s="4" t="s">
-        <v>135</v>
-      </c>
-      <c r="C18" s="4" t="s">
-        <v>147</v>
-      </c>
-      <c r="D18" s="4">
-        <v>27.121354681470969</v>
-      </c>
-      <c r="E18" s="4">
-        <v>69.927720542756759</v>
-      </c>
-      <c r="F18" s="4" t="s">
-        <v>148</v>
-      </c>
-      <c r="G18" s="1">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="19" spans="1:7">
+        <v>274</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6">
+      <c r="A17" s="16" t="s">
+        <v>259</v>
+      </c>
+      <c r="B17" s="16" t="s">
+        <v>256</v>
+      </c>
+      <c r="C17" s="22">
+        <v>69.445760000000007</v>
+      </c>
+      <c r="D17" s="22">
+        <v>25.355440000000002</v>
+      </c>
+      <c r="E17" s="7" t="s">
+        <v>196</v>
+      </c>
+      <c r="F17" s="7" t="s">
+        <v>275</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6">
+      <c r="A18" s="18" t="s">
+        <v>257</v>
+      </c>
+      <c r="B18" s="7" t="s">
+        <v>283</v>
+      </c>
+      <c r="C18" s="22">
+        <v>69.468090000000004</v>
+      </c>
+      <c r="D18" s="22">
+        <v>25.507429999999999</v>
+      </c>
+      <c r="E18" s="7" t="s">
+        <v>282</v>
+      </c>
+      <c r="F18" s="7" t="s">
+        <v>280</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6">
       <c r="A19" s="4" t="s">
         <v>136</v>
       </c>
       <c r="B19" s="4" t="s">
         <v>137</v>
       </c>
-      <c r="C19" s="4" t="s">
+      <c r="C19" s="23">
+        <v>69.472572555143302</v>
+      </c>
+      <c r="D19" s="23">
+        <v>25.85313273161557</v>
+      </c>
+      <c r="E19" s="4" t="s">
         <v>147</v>
       </c>
-      <c r="D19" s="4">
-        <v>25.85313273161557</v>
-      </c>
-      <c r="E19" s="4">
-        <v>69.472572555143302</v>
-      </c>
       <c r="F19" s="4" t="s">
-        <v>148</v>
-      </c>
-      <c r="G19" s="1">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="20" spans="1:7">
-      <c r="A20" s="4" t="s">
-        <v>138</v>
-      </c>
-      <c r="B20" s="4" t="s">
-        <v>139</v>
-      </c>
-      <c r="C20" s="4" t="s">
-        <v>147</v>
-      </c>
-      <c r="D20" s="4">
-        <v>28.19830818020764</v>
-      </c>
-      <c r="E20" s="4">
-        <v>70.195935132530565</v>
-      </c>
-      <c r="F20" s="4" t="s">
-        <v>148</v>
-      </c>
-      <c r="G20" s="1">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="21" spans="1:7">
-      <c r="A21" s="4" t="s">
-        <v>140</v>
-      </c>
-      <c r="B21" s="4" t="s">
-        <v>141</v>
-      </c>
-      <c r="C21" s="4" t="s">
-        <v>147</v>
-      </c>
-      <c r="D21" s="4">
-        <v>28.16908580439851</v>
-      </c>
-      <c r="E21" s="4">
-        <v>70.22968067182029</v>
-      </c>
-      <c r="F21" s="4" t="s">
-        <v>148</v>
-      </c>
-      <c r="G21" s="1">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="22" spans="1:7">
-      <c r="A22" s="4" t="s">
-        <v>142</v>
-      </c>
-      <c r="B22" s="4" t="s">
-        <v>143</v>
-      </c>
-      <c r="C22" s="4" t="s">
-        <v>147</v>
-      </c>
-      <c r="D22" s="4">
-        <v>27.720222929469681</v>
-      </c>
-      <c r="E22" s="4">
-        <v>70.069685304299611</v>
-      </c>
-      <c r="F22" s="4" t="s">
-        <v>148</v>
-      </c>
-      <c r="G22" s="1">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="23" spans="1:7">
+        <v>274</v>
+      </c>
+    </row>
+    <row r="20" spans="1:6">
+      <c r="A20" s="6" t="s">
+        <v>177</v>
+      </c>
+      <c r="B20" s="7" t="s">
+        <v>178</v>
+      </c>
+      <c r="C20" s="22">
+        <v>69.534884730000002</v>
+      </c>
+      <c r="D20" s="22">
+        <v>24.890296469999999</v>
+      </c>
+      <c r="E20" s="7" t="s">
+        <v>196</v>
+      </c>
+      <c r="F20" s="7" t="s">
+        <v>275</v>
+      </c>
+    </row>
+    <row r="21" spans="1:6">
+      <c r="A21" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="B21" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="C21" s="23">
+        <v>69.565611000000004</v>
+      </c>
+      <c r="D21" s="23">
+        <v>24.388183000000001</v>
+      </c>
+      <c r="E21" s="1" t="s">
+        <v>146</v>
+      </c>
+      <c r="F21" s="1" t="s">
+        <v>267</v>
+      </c>
+    </row>
+    <row r="22" spans="1:6">
+      <c r="A22" s="16" t="s">
+        <v>186</v>
+      </c>
+      <c r="B22" s="16" t="s">
+        <v>186</v>
+      </c>
+      <c r="C22" s="22">
+        <v>69.908649999999994</v>
+      </c>
+      <c r="D22" s="22">
+        <v>27.047160000000002</v>
+      </c>
+      <c r="E22" s="7" t="s">
+        <v>196</v>
+      </c>
+      <c r="F22" s="7" t="s">
+        <v>275</v>
+      </c>
+    </row>
+    <row r="23" spans="1:6">
       <c r="A23" s="4" t="s">
         <v>144</v>
       </c>
       <c r="B23" s="4" t="s">
         <v>145</v>
       </c>
-      <c r="C23" s="4" t="s">
+      <c r="C23" s="23">
+        <v>69.910494088438014</v>
+      </c>
+      <c r="D23" s="23">
+        <v>27.03387805245907</v>
+      </c>
+      <c r="E23" s="4" t="s">
         <v>147</v>
       </c>
-      <c r="D23" s="4">
-        <v>27.03387805245907</v>
-      </c>
-      <c r="E23" s="4">
-        <v>69.910494088438014</v>
-      </c>
       <c r="F23" s="4" t="s">
-        <v>148</v>
-      </c>
-      <c r="G23" s="1">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="24" spans="1:7">
-      <c r="A24" s="6">
-        <v>4</v>
-      </c>
-      <c r="B24" s="7" t="s">
-        <v>160</v>
-      </c>
-      <c r="C24" s="4" t="s">
+        <v>274</v>
+      </c>
+    </row>
+    <row r="24" spans="1:6">
+      <c r="A24" s="4" t="s">
+        <v>134</v>
+      </c>
+      <c r="B24" s="4" t="s">
+        <v>135</v>
+      </c>
+      <c r="C24" s="23">
+        <v>69.927720542756759</v>
+      </c>
+      <c r="D24" s="23">
+        <v>27.121354681470969</v>
+      </c>
+      <c r="E24" s="4" t="s">
         <v>147</v>
       </c>
-      <c r="D24" s="7">
-        <v>25.597493</v>
-      </c>
-      <c r="E24" s="7">
-        <v>68.926158000000001</v>
-      </c>
-      <c r="F24" s="7" t="s">
+      <c r="F24" s="4" t="s">
+        <v>274</v>
+      </c>
+    </row>
+    <row r="25" spans="1:6">
+      <c r="A25" s="1" t="s">
+        <v>78</v>
+      </c>
+      <c r="B25" s="1" t="s">
+        <v>79</v>
+      </c>
+      <c r="C25" s="23">
+        <v>69.944618000000006</v>
+      </c>
+      <c r="D25" s="23">
+        <v>26.485793000000001</v>
+      </c>
+      <c r="E25" s="1" t="s">
+        <v>146</v>
+      </c>
+      <c r="F25" t="s">
+        <v>270</v>
+      </c>
+    </row>
+    <row r="26" spans="1:6">
+      <c r="A26" s="6">
+        <v>8</v>
+      </c>
+      <c r="B26" s="7" t="s">
+        <v>161</v>
+      </c>
+      <c r="C26" s="22">
+        <v>69.958485800000005</v>
+      </c>
+      <c r="D26" s="22">
+        <v>26.862095</v>
+      </c>
+      <c r="E26" s="7" t="s">
+        <v>196</v>
+      </c>
+      <c r="F26" s="7" t="s">
+        <v>275</v>
+      </c>
+    </row>
+    <row r="27" spans="1:6">
+      <c r="A27" s="6" t="s">
+        <v>181</v>
+      </c>
+      <c r="B27" s="7" t="s">
+        <v>182</v>
+      </c>
+      <c r="C27" s="22">
+        <v>69.967677710000004</v>
+      </c>
+      <c r="D27" s="22">
+        <v>26.424932210000001</v>
+      </c>
+      <c r="E27" s="7" t="s">
+        <v>196</v>
+      </c>
+      <c r="F27" s="7" t="s">
+        <v>276</v>
+      </c>
+    </row>
+    <row r="28" spans="1:6">
+      <c r="A28" s="4" t="s">
+        <v>142</v>
+      </c>
+      <c r="B28" s="4" t="s">
+        <v>143</v>
+      </c>
+      <c r="C28" s="23">
+        <v>70.069685304299611</v>
+      </c>
+      <c r="D28" s="23">
+        <v>27.720222929469681</v>
+      </c>
+      <c r="E28" s="4" t="s">
+        <v>147</v>
+      </c>
+      <c r="F28" s="4" t="s">
+        <v>274</v>
+      </c>
+    </row>
+    <row r="29" spans="1:6">
+      <c r="A29" s="1" t="s">
         <v>198</v>
       </c>
-      <c r="G24" s="7">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="25" spans="1:7">
-      <c r="A25" s="6">
-        <v>8</v>
-      </c>
-      <c r="B25" s="7" t="s">
-        <v>163</v>
-      </c>
-      <c r="C25" s="4" t="s">
+      <c r="B29" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="C29" s="23">
+        <v>70.070346999999998</v>
+      </c>
+      <c r="D29" s="23">
+        <v>28.016017000000002</v>
+      </c>
+      <c r="E29" s="1" t="s">
+        <v>277</v>
+      </c>
+      <c r="F29" s="1" t="s">
+        <v>284</v>
+      </c>
+    </row>
+    <row r="30" spans="1:6">
+      <c r="A30" s="1" t="s">
+        <v>105</v>
+      </c>
+      <c r="B30" s="1" t="s">
+        <v>106</v>
+      </c>
+      <c r="C30" s="23">
+        <v>70.074292</v>
+      </c>
+      <c r="D30" s="23">
+        <v>27.705573000000001</v>
+      </c>
+      <c r="E30" s="1" t="s">
+        <v>146</v>
+      </c>
+      <c r="F30" s="1" t="s">
+        <v>272</v>
+      </c>
+    </row>
+    <row r="31" spans="1:6">
+      <c r="A31" s="1" t="s">
+        <v>84</v>
+      </c>
+      <c r="B31" s="1" t="s">
+        <v>85</v>
+      </c>
+      <c r="C31" s="23">
+        <v>70.166214999999994</v>
+      </c>
+      <c r="D31" s="23">
+        <v>28.22343</v>
+      </c>
+      <c r="E31" s="1" t="s">
+        <v>146</v>
+      </c>
+      <c r="F31" s="1" t="s">
+        <v>271</v>
+      </c>
+    </row>
+    <row r="32" spans="1:6">
+      <c r="A32" s="4" t="s">
+        <v>138</v>
+      </c>
+      <c r="B32" s="4" t="s">
+        <v>139</v>
+      </c>
+      <c r="C32" s="23">
+        <v>70.195935132530565</v>
+      </c>
+      <c r="D32" s="23">
+        <v>28.19830818020764</v>
+      </c>
+      <c r="E32" s="4" t="s">
         <v>147</v>
       </c>
-      <c r="D25" s="7">
-        <v>26.862095</v>
-      </c>
-      <c r="E25" s="7">
-        <v>69.958485800000005</v>
-      </c>
-      <c r="F25" s="7" t="s">
+      <c r="F32" s="4" t="s">
+        <v>274</v>
+      </c>
+    </row>
+    <row r="33" spans="1:6">
+      <c r="A33" s="4" t="s">
+        <v>140</v>
+      </c>
+      <c r="B33" s="4" t="s">
+        <v>141</v>
+      </c>
+      <c r="C33" s="23">
+        <v>70.22968067182029</v>
+      </c>
+      <c r="D33" s="23">
+        <v>28.16908580439851</v>
+      </c>
+      <c r="E33" s="4" t="s">
+        <v>147</v>
+      </c>
+      <c r="F33" s="4" t="s">
+        <v>274</v>
+      </c>
+    </row>
+    <row r="34" spans="1:6">
+      <c r="A34" s="1" t="s">
+        <v>91</v>
+      </c>
+      <c r="B34" s="1" t="s">
+        <v>92</v>
+      </c>
+      <c r="C34" s="23">
+        <v>70.375489999999999</v>
+      </c>
+      <c r="D34" s="23">
+        <v>28.249378</v>
+      </c>
+      <c r="E34" s="1" t="s">
+        <v>146</v>
+      </c>
+      <c r="F34" t="s">
+        <v>266</v>
+      </c>
+    </row>
+    <row r="35" spans="1:6">
+      <c r="A35" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="B35" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="C35" s="23">
+        <v>70.419150999999999</v>
+      </c>
+      <c r="D35" s="23">
+        <v>28.041376</v>
+      </c>
+      <c r="E35" s="1" t="s">
+        <v>146</v>
+      </c>
+      <c r="F35" s="1" t="s">
+        <v>267</v>
+      </c>
+    </row>
+    <row r="36" spans="1:6">
+      <c r="A36" s="2" t="s">
+        <v>99</v>
+      </c>
+      <c r="B36" s="2" t="s">
+        <v>100</v>
+      </c>
+      <c r="C36" s="25">
+        <v>70.472215000000006</v>
+      </c>
+      <c r="D36" s="25">
+        <v>28.824532000000001</v>
+      </c>
+      <c r="E36" s="1" t="s">
+        <v>146</v>
+      </c>
+      <c r="F36" s="2" t="s">
+        <v>268</v>
+      </c>
+    </row>
+  </sheetData>
+  <autoFilter ref="A1:F36" xr:uid="{2CF353F4-079D-49EA-982B-68B02FF1D592}">
+    <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:F36">
+      <sortCondition ref="C1:C36"/>
+    </sortState>
+  </autoFilter>
+  <phoneticPr fontId="3" type="noConversion"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5E17FA22-8B99-4F74-B869-E4F468961C2B}">
+  <sheetPr filterMode="1"/>
+  <dimension ref="A1:J35"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:F35"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <cols>
+    <col min="8" max="8" width="20.7109375" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="22.5703125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:10">
+      <c r="A1" t="s">
+        <v>2</v>
+      </c>
+      <c r="B1" t="s">
+        <v>3</v>
+      </c>
+      <c r="C1" t="s">
+        <v>5</v>
+      </c>
+      <c r="D1" t="s">
+        <v>6</v>
+      </c>
+      <c r="E1" t="s">
+        <v>22</v>
+      </c>
+      <c r="F1" t="s">
+        <v>23</v>
+      </c>
+      <c r="G1" t="s">
+        <v>207</v>
+      </c>
+      <c r="H1" t="s">
+        <v>234</v>
+      </c>
+      <c r="I1" t="s">
+        <v>238</v>
+      </c>
+      <c r="J1" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="2" spans="1:10">
+      <c r="A2" t="s">
+        <v>26</v>
+      </c>
+      <c r="B2" t="s">
+        <v>27</v>
+      </c>
+      <c r="C2">
+        <v>1003</v>
+      </c>
+      <c r="D2" t="s">
+        <v>75</v>
+      </c>
+      <c r="E2">
+        <v>24.474238</v>
+      </c>
+      <c r="F2">
+        <v>69.390030999999993</v>
+      </c>
+      <c r="G2">
+        <v>1</v>
+      </c>
+      <c r="H2">
+        <v>1</v>
+      </c>
+      <c r="J2" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="3" spans="1:10">
+      <c r="A3" t="s">
+        <v>26</v>
+      </c>
+      <c r="B3" t="s">
+        <v>27</v>
+      </c>
+      <c r="C3">
+        <v>1001</v>
+      </c>
+      <c r="D3" t="s">
+        <v>28</v>
+      </c>
+      <c r="E3">
+        <v>24.474238</v>
+      </c>
+      <c r="F3">
+        <v>69.390030999999993</v>
+      </c>
+      <c r="G3">
+        <v>1</v>
+      </c>
+      <c r="H3">
+        <v>1</v>
+      </c>
+      <c r="J3" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="4" spans="1:10">
+      <c r="A4" t="s">
+        <v>91</v>
+      </c>
+      <c r="B4" t="s">
+        <v>92</v>
+      </c>
+      <c r="C4">
+        <v>2000</v>
+      </c>
+      <c r="D4" t="s">
+        <v>93</v>
+      </c>
+      <c r="E4">
+        <v>28.249378</v>
+      </c>
+      <c r="F4">
+        <v>70.375489999999999</v>
+      </c>
+      <c r="G4">
+        <v>1</v>
+      </c>
+      <c r="H4">
+        <v>1</v>
+      </c>
+      <c r="J4" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="5" spans="1:10">
+      <c r="A5" t="s">
+        <v>91</v>
+      </c>
+      <c r="B5" t="s">
+        <v>92</v>
+      </c>
+      <c r="C5">
+        <v>2015</v>
+      </c>
+      <c r="D5" t="s">
+        <v>211</v>
+      </c>
+      <c r="E5">
+        <v>28.249378</v>
+      </c>
+      <c r="F5">
+        <v>70.375489999999999</v>
+      </c>
+      <c r="G5">
+        <v>1</v>
+      </c>
+      <c r="H5">
+        <v>1</v>
+      </c>
+      <c r="J5" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="6" spans="1:10">
+      <c r="A6" t="s">
+        <v>36</v>
+      </c>
+      <c r="B6" t="s">
+        <v>37</v>
+      </c>
+      <c r="C6">
+        <v>1001</v>
+      </c>
+      <c r="D6" t="s">
+        <v>28</v>
+      </c>
+      <c r="E6">
+        <v>24.388183000000001</v>
+      </c>
+      <c r="F6">
+        <v>69.565611000000004</v>
+      </c>
+      <c r="G6">
+        <v>1</v>
+      </c>
+      <c r="H6">
+        <v>1</v>
+      </c>
+      <c r="J6" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="7" spans="1:10">
+      <c r="A7" s="8" t="s">
+        <v>99</v>
+      </c>
+      <c r="B7" s="8" t="s">
+        <v>100</v>
+      </c>
+      <c r="C7" s="8">
+        <v>1001</v>
+      </c>
+      <c r="D7" s="8" t="s">
+        <v>28</v>
+      </c>
+      <c r="E7" s="8">
+        <v>28.824532000000001</v>
+      </c>
+      <c r="F7" s="8">
+        <v>70.472215000000006</v>
+      </c>
+      <c r="G7" s="8">
+        <v>1</v>
+      </c>
+      <c r="H7" s="8">
+        <v>1</v>
+      </c>
+      <c r="I7" s="8"/>
+      <c r="J7" s="8" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="8" spans="1:10">
+      <c r="A8" s="8" t="s">
+        <v>99</v>
+      </c>
+      <c r="B8" s="8" t="s">
+        <v>100</v>
+      </c>
+      <c r="C8" s="8">
+        <v>1208</v>
+      </c>
+      <c r="D8" s="8" t="s">
+        <v>107</v>
+      </c>
+      <c r="E8" s="8">
+        <v>28.824532000000001</v>
+      </c>
+      <c r="F8" s="8">
+        <v>70.472215000000006</v>
+      </c>
+      <c r="G8" s="8">
+        <v>1</v>
+      </c>
+      <c r="H8" s="8">
+        <v>1</v>
+      </c>
+      <c r="I8" s="8"/>
+      <c r="J8" s="8" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="9" spans="1:10">
+      <c r="A9" s="8" t="s">
+        <v>99</v>
+      </c>
+      <c r="B9" s="8" t="s">
+        <v>100</v>
+      </c>
+      <c r="C9" s="8">
+        <v>1200</v>
+      </c>
+      <c r="D9" s="8" t="s">
+        <v>215</v>
+      </c>
+      <c r="E9" s="8">
+        <v>28.824532000000001</v>
+      </c>
+      <c r="F9" s="8">
+        <v>70.472215000000006</v>
+      </c>
+      <c r="G9" s="8">
+        <v>1</v>
+      </c>
+      <c r="H9" s="8">
+        <v>1</v>
+      </c>
+      <c r="I9" s="8"/>
+      <c r="J9" s="8" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="10" spans="1:10">
+      <c r="A10" t="s">
+        <v>66</v>
+      </c>
+      <c r="B10" t="s">
+        <v>67</v>
+      </c>
+      <c r="C10">
+        <v>1000</v>
+      </c>
+      <c r="D10" t="s">
+        <v>68</v>
+      </c>
+      <c r="E10">
+        <v>25.510739000000001</v>
+      </c>
+      <c r="F10">
+        <v>69.469237000000007</v>
+      </c>
+      <c r="G10">
+        <v>1</v>
+      </c>
+      <c r="H10">
+        <v>1</v>
+      </c>
+      <c r="J10" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="11" spans="1:10">
+      <c r="A11" t="s">
+        <v>66</v>
+      </c>
+      <c r="B11" t="s">
+        <v>67</v>
+      </c>
+      <c r="C11">
+        <v>1003</v>
+      </c>
+      <c r="D11" t="s">
+        <v>75</v>
+      </c>
+      <c r="E11">
+        <v>25.510739000000001</v>
+      </c>
+      <c r="F11">
+        <v>69.469237000000007</v>
+      </c>
+      <c r="G11">
+        <v>1</v>
+      </c>
+      <c r="H11">
+        <v>1</v>
+      </c>
+      <c r="J11" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="12" spans="1:10" hidden="1">
+      <c r="A12" t="s">
+        <v>201</v>
+      </c>
+      <c r="B12" t="s">
+        <v>202</v>
+      </c>
+      <c r="C12">
+        <v>2000</v>
+      </c>
+      <c r="D12" t="s">
+        <v>93</v>
+      </c>
+      <c r="E12">
+        <v>25.815045999999999</v>
+      </c>
+      <c r="F12">
+        <v>69.400755000000004</v>
+      </c>
+      <c r="G12">
+        <v>1</v>
+      </c>
+      <c r="H12">
+        <v>0</v>
+      </c>
+      <c r="J12" t="s">
+        <v>235</v>
+      </c>
+    </row>
+    <row r="13" spans="1:10" hidden="1">
+      <c r="A13" t="s">
+        <v>201</v>
+      </c>
+      <c r="B13" t="s">
+        <v>202</v>
+      </c>
+      <c r="C13">
+        <v>2015</v>
+      </c>
+      <c r="D13" t="s">
+        <v>211</v>
+      </c>
+      <c r="E13">
+        <v>25.815045999999999</v>
+      </c>
+      <c r="F13">
+        <v>69.400755000000004</v>
+      </c>
+      <c r="G13">
+        <v>1</v>
+      </c>
+      <c r="H13">
+        <v>0</v>
+      </c>
+      <c r="J13" t="s">
+        <v>235</v>
+      </c>
+    </row>
+    <row r="14" spans="1:10" hidden="1">
+      <c r="A14" t="s">
+        <v>203</v>
+      </c>
+      <c r="B14" t="s">
+        <v>204</v>
+      </c>
+      <c r="C14">
+        <v>2000</v>
+      </c>
+      <c r="D14" t="s">
+        <v>93</v>
+      </c>
+      <c r="E14">
+        <v>25.814402000000001</v>
+      </c>
+      <c r="F14">
+        <v>69.400858999999997</v>
+      </c>
+      <c r="G14">
+        <v>1</v>
+      </c>
+      <c r="H14">
+        <v>0</v>
+      </c>
+      <c r="J14" t="s">
+        <v>235</v>
+      </c>
+    </row>
+    <row r="15" spans="1:10">
+      <c r="A15" t="s">
+        <v>205</v>
+      </c>
+      <c r="B15" t="s">
+        <v>206</v>
+      </c>
+      <c r="C15">
+        <v>2006</v>
+      </c>
+      <c r="D15" t="s">
+        <v>209</v>
+      </c>
+      <c r="E15">
+        <v>25.814402000000001</v>
+      </c>
+      <c r="F15">
+        <v>69.400858999999997</v>
+      </c>
+      <c r="G15">
+        <v>1</v>
+      </c>
+      <c r="H15">
+        <v>1</v>
+      </c>
+      <c r="J15" t="s">
+        <v>235</v>
+      </c>
+    </row>
+    <row r="16" spans="1:10">
+      <c r="A16" t="s">
+        <v>205</v>
+      </c>
+      <c r="B16" t="s">
+        <v>206</v>
+      </c>
+      <c r="C16">
+        <v>2015</v>
+      </c>
+      <c r="D16" t="s">
+        <v>211</v>
+      </c>
+      <c r="E16">
+        <v>25.814402000000001</v>
+      </c>
+      <c r="F16">
+        <v>69.400858999999997</v>
+      </c>
+      <c r="G16">
+        <v>1</v>
+      </c>
+      <c r="H16">
+        <v>1</v>
+      </c>
+      <c r="J16" t="s">
+        <v>235</v>
+      </c>
+    </row>
+    <row r="17" spans="1:10">
+      <c r="A17" t="s">
+        <v>205</v>
+      </c>
+      <c r="B17" t="s">
+        <v>206</v>
+      </c>
+      <c r="C17">
+        <v>2001</v>
+      </c>
+      <c r="D17" t="s">
+        <v>216</v>
+      </c>
+      <c r="E17">
+        <v>25.814402000000001</v>
+      </c>
+      <c r="F17">
+        <v>69.400858999999997</v>
+      </c>
+      <c r="G17">
+        <v>1</v>
+      </c>
+      <c r="H17">
+        <v>1</v>
+      </c>
+      <c r="J17" t="s">
+        <v>235</v>
+      </c>
+    </row>
+    <row r="18" spans="1:10">
+      <c r="A18" t="s">
+        <v>205</v>
+      </c>
+      <c r="B18" t="s">
+        <v>206</v>
+      </c>
+      <c r="C18">
+        <v>2000</v>
+      </c>
+      <c r="D18" t="s">
+        <v>93</v>
+      </c>
+      <c r="E18">
+        <v>25.814402000000001</v>
+      </c>
+      <c r="F18">
+        <v>69.400858999999997</v>
+      </c>
+      <c r="G18">
+        <v>1</v>
+      </c>
+      <c r="H18">
+        <v>1</v>
+      </c>
+      <c r="J18" t="s">
+        <v>235</v>
+      </c>
+    </row>
+    <row r="19" spans="1:10">
+      <c r="A19" t="s">
+        <v>78</v>
+      </c>
+      <c r="B19" t="s">
+        <v>79</v>
+      </c>
+      <c r="C19">
+        <v>1000</v>
+      </c>
+      <c r="D19" t="s">
+        <v>68</v>
+      </c>
+      <c r="E19">
+        <v>26.485793000000001</v>
+      </c>
+      <c r="F19">
+        <v>69.944618000000006</v>
+      </c>
+      <c r="G19">
+        <v>1</v>
+      </c>
+      <c r="H19">
+        <v>1</v>
+      </c>
+      <c r="J19" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="20" spans="1:10">
+      <c r="A20" t="s">
+        <v>42</v>
+      </c>
+      <c r="B20" t="s">
+        <v>43</v>
+      </c>
+      <c r="C20">
+        <v>1001</v>
+      </c>
+      <c r="D20" t="s">
+        <v>28</v>
+      </c>
+      <c r="E20">
+        <v>25.158322999999999</v>
+      </c>
+      <c r="F20">
+        <v>69.419317000000007</v>
+      </c>
+      <c r="G20">
+        <v>1</v>
+      </c>
+      <c r="H20">
+        <v>1</v>
+      </c>
+      <c r="J20" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="21" spans="1:10" hidden="1">
+      <c r="A21" t="s">
+        <v>197</v>
+      </c>
+      <c r="B21" t="s">
         <v>198</v>
       </c>
-      <c r="G25" s="7">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="26" spans="1:7">
-      <c r="A26" s="6">
-        <v>12</v>
-      </c>
-      <c r="B26" s="7" t="s">
-        <v>168</v>
-      </c>
-      <c r="C26" s="4" t="s">
-        <v>147</v>
-      </c>
-      <c r="D26" s="7">
-        <v>25.098504399999999</v>
-      </c>
-      <c r="E26" s="7">
-        <v>69.338290299999997</v>
-      </c>
-      <c r="F26" s="7" t="s">
-        <v>198</v>
-      </c>
-      <c r="G26" s="7">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="27" spans="1:7">
-      <c r="A27" s="6">
-        <v>13</v>
-      </c>
-      <c r="B27" s="7" t="s">
-        <v>169</v>
-      </c>
-      <c r="C27" s="4" t="s">
-        <v>147</v>
-      </c>
-      <c r="D27" s="7">
-        <v>25.7197402</v>
-      </c>
-      <c r="E27" s="7">
-        <v>69.106753400000002</v>
-      </c>
-      <c r="F27" s="7" t="s">
-        <v>198</v>
-      </c>
-      <c r="G27" s="7">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="28" spans="1:7">
-      <c r="A28" s="6">
-        <v>14</v>
-      </c>
-      <c r="B28" s="7" t="s">
-        <v>172</v>
-      </c>
-      <c r="C28" s="4" t="s">
-        <v>147</v>
-      </c>
-      <c r="D28" s="7">
-        <v>24.472635199999999</v>
-      </c>
-      <c r="E28" s="7">
-        <v>69.38992184</v>
-      </c>
-      <c r="F28" s="7" t="s">
-        <v>198</v>
-      </c>
-      <c r="G28" s="7">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="29" spans="1:7">
-      <c r="A29" s="6" t="s">
-        <v>170</v>
-      </c>
-      <c r="B29" s="7" t="s">
-        <v>171</v>
-      </c>
-      <c r="C29" s="4" t="s">
-        <v>147</v>
-      </c>
-      <c r="D29" s="7">
-        <v>25.689412659999999</v>
-      </c>
-      <c r="E29" s="7">
-        <v>69.199913890000005</v>
-      </c>
-      <c r="F29" s="7" t="s">
-        <v>198</v>
-      </c>
-      <c r="G29" s="7">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="30" spans="1:7">
-      <c r="A30" s="6" t="s">
-        <v>177</v>
-      </c>
-      <c r="B30" s="7" t="s">
-        <v>178</v>
-      </c>
-      <c r="C30" s="4" t="s">
-        <v>147</v>
-      </c>
-      <c r="D30" s="7">
-        <v>24.010010829999999</v>
-      </c>
-      <c r="E30" s="7">
-        <v>69.327241860000001</v>
-      </c>
-      <c r="F30" s="7" t="s">
-        <v>198</v>
-      </c>
-      <c r="G30" s="7">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="31" spans="1:7">
-      <c r="A31" s="6" t="s">
-        <v>179</v>
-      </c>
-      <c r="B31" s="7" t="s">
-        <v>180</v>
-      </c>
-      <c r="C31" s="4" t="s">
-        <v>147</v>
-      </c>
-      <c r="D31" s="7">
-        <v>24.890296469999999</v>
-      </c>
-      <c r="E31" s="7">
-        <v>69.534884730000002</v>
-      </c>
-      <c r="F31" s="7" t="s">
-        <v>198</v>
-      </c>
-      <c r="G31" s="7">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="32" spans="1:7">
-      <c r="A32" s="6" t="s">
-        <v>183</v>
-      </c>
-      <c r="B32" s="7" t="s">
-        <v>184</v>
-      </c>
-      <c r="C32" s="4" t="s">
-        <v>147</v>
-      </c>
-      <c r="D32" s="7">
-        <v>26.424932210000001</v>
-      </c>
-      <c r="E32" s="7">
-        <v>69.967677710000004</v>
-      </c>
-      <c r="F32" s="7" t="s">
-        <v>198</v>
-      </c>
-      <c r="G32" s="7">
-        <v>0</v>
+      <c r="C21">
+        <v>1001</v>
+      </c>
+      <c r="D21" t="s">
+        <v>28</v>
+      </c>
+      <c r="E21">
+        <v>28.057406</v>
+      </c>
+      <c r="F21">
+        <v>70.072616999999994</v>
+      </c>
+      <c r="G21">
+        <v>1</v>
+      </c>
+      <c r="H21">
+        <v>0</v>
+      </c>
+      <c r="I21" t="s">
+        <v>48</v>
+      </c>
+      <c r="J21" t="s">
+        <v>229</v>
+      </c>
+    </row>
+    <row r="22" spans="1:10">
+      <c r="A22" t="s">
+        <v>48</v>
+      </c>
+      <c r="B22" t="s">
+        <v>49</v>
+      </c>
+      <c r="C22">
+        <v>1200</v>
+      </c>
+      <c r="D22" t="s">
+        <v>215</v>
+      </c>
+      <c r="E22">
+        <v>28.016017000000002</v>
+      </c>
+      <c r="F22">
+        <v>70.070346999999998</v>
+      </c>
+      <c r="G22">
+        <v>1</v>
+      </c>
+      <c r="H22">
+        <v>1</v>
+      </c>
+      <c r="J22" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="23" spans="1:10">
+      <c r="A23" t="s">
+        <v>48</v>
+      </c>
+      <c r="B23" t="s">
+        <v>49</v>
+      </c>
+      <c r="C23">
+        <v>1208</v>
+      </c>
+      <c r="D23" t="s">
+        <v>107</v>
+      </c>
+      <c r="E23">
+        <v>28.016017000000002</v>
+      </c>
+      <c r="F23">
+        <v>70.070346999999998</v>
+      </c>
+      <c r="G23">
+        <v>1</v>
+      </c>
+      <c r="H23">
+        <v>1</v>
+      </c>
+      <c r="J23" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="24" spans="1:10">
+      <c r="A24" t="s">
+        <v>48</v>
+      </c>
+      <c r="B24" t="s">
+        <v>49</v>
+      </c>
+      <c r="C24">
+        <v>1001</v>
+      </c>
+      <c r="D24" t="s">
+        <v>28</v>
+      </c>
+      <c r="E24">
+        <v>28.016017000000002</v>
+      </c>
+      <c r="F24">
+        <v>70.070346999999998</v>
+      </c>
+      <c r="G24">
+        <v>1</v>
+      </c>
+      <c r="H24">
+        <v>1</v>
+      </c>
+      <c r="J24" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="25" spans="1:10">
+      <c r="A25" t="s">
+        <v>48</v>
+      </c>
+      <c r="B25" t="s">
+        <v>49</v>
+      </c>
+      <c r="C25">
+        <v>1003</v>
+      </c>
+      <c r="D25" t="s">
+        <v>75</v>
+      </c>
+      <c r="E25">
+        <v>28.016017000000002</v>
+      </c>
+      <c r="F25">
+        <v>70.070346999999998</v>
+      </c>
+      <c r="G25">
+        <v>1</v>
+      </c>
+      <c r="H25">
+        <v>1</v>
+      </c>
+      <c r="J25" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="26" spans="1:10">
+      <c r="A26" t="s">
+        <v>84</v>
+      </c>
+      <c r="B26" t="s">
+        <v>85</v>
+      </c>
+      <c r="C26">
+        <v>2002</v>
+      </c>
+      <c r="D26" t="s">
+        <v>214</v>
+      </c>
+      <c r="E26">
+        <v>28.22343</v>
+      </c>
+      <c r="F26">
+        <v>70.166214999999994</v>
+      </c>
+      <c r="G26">
+        <v>1</v>
+      </c>
+      <c r="H26">
+        <v>1</v>
+      </c>
+      <c r="J26" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="27" spans="1:10">
+      <c r="A27" t="s">
+        <v>52</v>
+      </c>
+      <c r="B27" t="s">
+        <v>53</v>
+      </c>
+      <c r="C27">
+        <v>1001</v>
+      </c>
+      <c r="D27" t="s">
+        <v>28</v>
+      </c>
+      <c r="E27">
+        <v>28.041376</v>
+      </c>
+      <c r="F27">
+        <v>70.419150999999999</v>
+      </c>
+      <c r="G27">
+        <v>1</v>
+      </c>
+      <c r="H27">
+        <v>1</v>
+      </c>
+      <c r="J27" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="28" spans="1:10" hidden="1">
+      <c r="A28" t="s">
+        <v>217</v>
+      </c>
+      <c r="B28" t="s">
+        <v>218</v>
+      </c>
+      <c r="C28">
+        <v>1003</v>
+      </c>
+      <c r="D28" t="s">
+        <v>75</v>
+      </c>
+      <c r="E28">
+        <v>27.78257</v>
+      </c>
+      <c r="F28">
+        <v>70.070637000000005</v>
+      </c>
+      <c r="G28">
+        <v>1</v>
+      </c>
+      <c r="H28">
+        <v>0</v>
+      </c>
+      <c r="I28" t="s">
+        <v>105</v>
+      </c>
+      <c r="J28" t="s">
+        <v>237</v>
+      </c>
+    </row>
+    <row r="29" spans="1:10" hidden="1">
+      <c r="A29" t="s">
+        <v>219</v>
+      </c>
+      <c r="B29" t="s">
+        <v>220</v>
+      </c>
+      <c r="C29">
+        <v>1003</v>
+      </c>
+      <c r="D29" t="s">
+        <v>75</v>
+      </c>
+      <c r="E29">
+        <v>28.055733</v>
+      </c>
+      <c r="F29">
+        <v>70.072055000000006</v>
+      </c>
+      <c r="G29">
+        <v>1</v>
+      </c>
+      <c r="H29">
+        <v>0</v>
+      </c>
+      <c r="I29" t="s">
+        <v>48</v>
+      </c>
+      <c r="J29" t="s">
+        <v>239</v>
+      </c>
+    </row>
+    <row r="30" spans="1:10">
+      <c r="A30" t="s">
+        <v>105</v>
+      </c>
+      <c r="B30" t="s">
+        <v>106</v>
+      </c>
+      <c r="C30">
+        <v>1200</v>
+      </c>
+      <c r="D30" t="s">
+        <v>215</v>
+      </c>
+      <c r="E30">
+        <v>27.705573000000001</v>
+      </c>
+      <c r="F30">
+        <v>70.074292</v>
+      </c>
+      <c r="G30">
+        <v>1</v>
+      </c>
+      <c r="H30">
+        <v>1</v>
+      </c>
+      <c r="J30" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="31" spans="1:10">
+      <c r="A31" t="s">
+        <v>105</v>
+      </c>
+      <c r="B31" t="s">
+        <v>106</v>
+      </c>
+      <c r="C31">
+        <v>1208</v>
+      </c>
+      <c r="D31" t="s">
+        <v>107</v>
+      </c>
+      <c r="E31">
+        <v>27.705573000000001</v>
+      </c>
+      <c r="F31">
+        <v>70.074292</v>
+      </c>
+      <c r="G31">
+        <v>1</v>
+      </c>
+      <c r="H31">
+        <v>1</v>
+      </c>
+      <c r="J31" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="32" spans="1:10">
+      <c r="A32" t="s">
+        <v>57</v>
+      </c>
+      <c r="B32" t="s">
+        <v>58</v>
+      </c>
+      <c r="C32">
+        <v>1001</v>
+      </c>
+      <c r="D32" t="s">
+        <v>28</v>
+      </c>
+      <c r="E32">
+        <v>24.938338000000002</v>
+      </c>
+      <c r="F32">
+        <v>69.426393000000004</v>
+      </c>
+      <c r="G32">
+        <v>1</v>
+      </c>
+      <c r="H32">
+        <v>1</v>
+      </c>
+      <c r="J32" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="33" spans="1:10">
+      <c r="A33" t="s">
+        <v>57</v>
+      </c>
+      <c r="B33" t="s">
+        <v>58</v>
+      </c>
+      <c r="C33">
+        <v>1003</v>
+      </c>
+      <c r="D33" t="s">
+        <v>75</v>
+      </c>
+      <c r="E33">
+        <v>24.938338000000002</v>
+      </c>
+      <c r="F33">
+        <v>69.426393000000004</v>
+      </c>
+      <c r="G33">
+        <v>1</v>
+      </c>
+      <c r="H33">
+        <v>1</v>
+      </c>
+      <c r="J33" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="34" spans="1:10" hidden="1">
+      <c r="A34" t="s">
+        <v>199</v>
+      </c>
+      <c r="B34" t="s">
+        <v>200</v>
+      </c>
+      <c r="C34">
+        <v>1001</v>
+      </c>
+      <c r="D34" t="s">
+        <v>28</v>
+      </c>
+      <c r="E34">
+        <v>24.945211</v>
+      </c>
+      <c r="F34">
+        <v>69.427194</v>
+      </c>
+      <c r="G34">
+        <v>1</v>
+      </c>
+      <c r="H34">
+        <v>0</v>
+      </c>
+      <c r="I34" t="s">
+        <v>57</v>
+      </c>
+      <c r="J34" t="s">
+        <v>233</v>
+      </c>
+    </row>
+    <row r="35" spans="1:10">
+      <c r="A35" t="s">
+        <v>73</v>
+      </c>
+      <c r="B35" t="s">
+        <v>74</v>
+      </c>
+      <c r="C35">
+        <v>2000</v>
+      </c>
+      <c r="D35" t="s">
+        <v>93</v>
+      </c>
+      <c r="E35">
+        <v>25.811848999999999</v>
+      </c>
+      <c r="F35">
+        <v>69.408237</v>
+      </c>
+      <c r="G35">
+        <v>1</v>
+      </c>
+      <c r="H35">
+        <v>1</v>
+      </c>
+      <c r="J35" t="s">
+        <v>236</v>
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:G32" xr:uid="{AA1A77BB-F3C4-4B9E-9EDE-EEB6967A7FE8}"/>
-  <phoneticPr fontId="3" type="noConversion"/>
+  <autoFilter ref="A1:AB35" xr:uid="{FFFD35B6-2FA8-40AC-A5C6-3E4817891152}">
+    <filterColumn colId="7">
+      <filters>
+        <filter val="1"/>
+      </filters>
+    </filterColumn>
+  </autoFilter>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Consolidate some of the points for delineating catchments
</commit_message>
<xml_diff>
--- a/data/subcatchments_metadata/Subcatchments_existing_data_metadata.xlsx
+++ b/data/subcatchments_metadata/Subcatchments_existing_data_metadata.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Data\GitHub\quantom\data\subcatchments_metadata\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A0D2A7BB-28A5-4FC8-BDB2-F54B0CF41F19}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FBEF3F47-0A40-4F49-9267-BB3D7757B1BE}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17640" activeTab="5" xr2:uid="{3F73A599-D124-4158-BF3B-2BBEA0E40BC3}"/>
   </bookViews>
@@ -19,13 +19,11 @@
     <sheet name="quantom_2022_sensors" sheetId="13" r:id="rId4"/>
     <sheet name="Manual_SC_points" sheetId="12" r:id="rId5"/>
     <sheet name="Summary_all_points" sheetId="4" r:id="rId6"/>
-    <sheet name="Sheet1" sheetId="14" r:id="rId7"/>
   </sheets>
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Hydrol!$A$1:$E$14</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="2" hidden="1">Quantom_SCs!$A$1:$J$22</definedName>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="6" hidden="1">Sheet1!$A$1:$AB$35</definedName>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="5" hidden="1">Summary_all_points!$A$1:$F$36</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="5" hidden="1">Summary_all_points!$A$1:$F$35</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -43,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="951" uniqueCount="285">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="797" uniqueCount="287">
   <si>
     <t>objektType</t>
   </si>
@@ -861,9 +859,6 @@
     <t>Snow depth</t>
   </si>
   <si>
-    <t>SS</t>
-  </si>
-  <si>
     <t>Groundwater level</t>
   </si>
   <si>
@@ -898,6 +893,15 @@
   </si>
   <si>
     <t>Discharge, water temp, SS (NVE), Sensor and chem (Quantom)</t>
+  </si>
+  <si>
+    <t>NVE, Vannmiljø</t>
+  </si>
+  <si>
+    <t>SS, water chem</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Tana v/Storfossen &amp; Jalvvivárri </t>
   </si>
 </sst>
 </file>
@@ -4875,7 +4879,7 @@
   <dimension ref="A1:H34"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A5" sqref="A5:E29"/>
+      <selection activeCell="B29" sqref="B5:B29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -5725,7 +5729,7 @@
   <dimension ref="A1:G3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:D3"/>
+      <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -5795,10 +5799,10 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B293E105-2DEC-4AB0-8F8B-0F0216933BBC}">
-  <dimension ref="A1:F36"/>
+  <dimension ref="A1:F35"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D21" sqref="D21"/>
+      <selection activeCell="I17" sqref="I17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -5846,7 +5850,7 @@
         <v>196</v>
       </c>
       <c r="F2" s="7" t="s">
-        <v>275</v>
+        <v>274</v>
       </c>
     </row>
     <row r="3" spans="1:6" s="1" customFormat="1">
@@ -5866,7 +5870,7 @@
         <v>196</v>
       </c>
       <c r="F3" s="7" t="s">
-        <v>275</v>
+        <v>274</v>
       </c>
     </row>
     <row r="4" spans="1:6" s="1" customFormat="1">
@@ -5886,7 +5890,7 @@
         <v>196</v>
       </c>
       <c r="F4" s="7" t="s">
-        <v>276</v>
+        <v>275</v>
       </c>
     </row>
     <row r="5" spans="1:6" s="1" customFormat="1">
@@ -5906,7 +5910,7 @@
         <v>196</v>
       </c>
       <c r="F5" s="7" t="s">
-        <v>276</v>
+        <v>275</v>
       </c>
     </row>
     <row r="6" spans="1:6" s="1" customFormat="1">
@@ -5926,7 +5930,7 @@
         <v>196</v>
       </c>
       <c r="F6" s="7" t="s">
-        <v>275</v>
+        <v>274</v>
       </c>
     </row>
     <row r="7" spans="1:6" s="1" customFormat="1">
@@ -5946,7 +5950,7 @@
         <v>147</v>
       </c>
       <c r="F7" s="4" t="s">
-        <v>274</v>
+        <v>273</v>
       </c>
     </row>
     <row r="8" spans="1:6" s="1" customFormat="1">
@@ -5963,10 +5967,10 @@
         <v>24.472635199999999</v>
       </c>
       <c r="E8" s="7" t="s">
+        <v>276</v>
+      </c>
+      <c r="F8" s="7" t="s">
         <v>277</v>
-      </c>
-      <c r="F8" s="7" t="s">
-        <v>278</v>
       </c>
     </row>
     <row r="9" spans="1:6" s="1" customFormat="1">
@@ -5986,7 +5990,7 @@
         <v>196</v>
       </c>
       <c r="F9" s="7" t="s">
-        <v>276</v>
+        <v>275</v>
       </c>
     </row>
     <row r="10" spans="1:6" s="1" customFormat="1">
@@ -6026,7 +6030,7 @@
         <v>146</v>
       </c>
       <c r="F11" s="1" t="s">
-        <v>273</v>
+        <v>272</v>
       </c>
     </row>
     <row r="12" spans="1:6" s="1" customFormat="1">
@@ -6043,15 +6047,15 @@
         <v>25.159690000000001</v>
       </c>
       <c r="E12" s="7" t="s">
-        <v>277</v>
+        <v>276</v>
       </c>
       <c r="F12" s="7" t="s">
-        <v>279</v>
+        <v>278</v>
       </c>
     </row>
     <row r="13" spans="1:6" s="1" customFormat="1">
       <c r="A13" s="17" t="s">
-        <v>281</v>
+        <v>280</v>
       </c>
       <c r="B13" s="18" t="s">
         <v>260</v>
@@ -6063,10 +6067,10 @@
         <v>24.940829999999998</v>
       </c>
       <c r="E13" s="7" t="s">
-        <v>277</v>
+        <v>276</v>
       </c>
       <c r="F13" s="7" t="s">
-        <v>280</v>
+        <v>279</v>
       </c>
     </row>
     <row r="14" spans="1:6">
@@ -6106,7 +6110,7 @@
         <v>147</v>
       </c>
       <c r="F15" s="4" t="s">
-        <v>274</v>
+        <v>273</v>
       </c>
     </row>
     <row r="16" spans="1:6">
@@ -6126,7 +6130,7 @@
         <v>147</v>
       </c>
       <c r="F16" s="4" t="s">
-        <v>274</v>
+        <v>273</v>
       </c>
     </row>
     <row r="17" spans="1:6">
@@ -6146,7 +6150,7 @@
         <v>196</v>
       </c>
       <c r="F17" s="7" t="s">
-        <v>275</v>
+        <v>274</v>
       </c>
     </row>
     <row r="18" spans="1:6">
@@ -6154,7 +6158,7 @@
         <v>257</v>
       </c>
       <c r="B18" s="7" t="s">
-        <v>283</v>
+        <v>282</v>
       </c>
       <c r="C18" s="22">
         <v>69.468090000000004</v>
@@ -6163,10 +6167,10 @@
         <v>25.507429999999999</v>
       </c>
       <c r="E18" s="7" t="s">
-        <v>282</v>
+        <v>281</v>
       </c>
       <c r="F18" s="7" t="s">
-        <v>280</v>
+        <v>279</v>
       </c>
     </row>
     <row r="19" spans="1:6">
@@ -6186,7 +6190,7 @@
         <v>147</v>
       </c>
       <c r="F19" s="4" t="s">
-        <v>274</v>
+        <v>273</v>
       </c>
     </row>
     <row r="20" spans="1:6">
@@ -6206,7 +6210,7 @@
         <v>196</v>
       </c>
       <c r="F20" s="7" t="s">
-        <v>275</v>
+        <v>274</v>
       </c>
     </row>
     <row r="21" spans="1:6">
@@ -6246,7 +6250,7 @@
         <v>196</v>
       </c>
       <c r="F22" s="7" t="s">
-        <v>275</v>
+        <v>274</v>
       </c>
     </row>
     <row r="23" spans="1:6">
@@ -6266,7 +6270,7 @@
         <v>147</v>
       </c>
       <c r="F23" s="4" t="s">
-        <v>274</v>
+        <v>273</v>
       </c>
     </row>
     <row r="24" spans="1:6">
@@ -6286,7 +6290,7 @@
         <v>147</v>
       </c>
       <c r="F24" s="4" t="s">
-        <v>274</v>
+        <v>273</v>
       </c>
     </row>
     <row r="25" spans="1:6">
@@ -6326,7 +6330,7 @@
         <v>196</v>
       </c>
       <c r="F26" s="7" t="s">
-        <v>275</v>
+        <v>274</v>
       </c>
     </row>
     <row r="27" spans="1:6">
@@ -6346,1257 +6350,177 @@
         <v>196</v>
       </c>
       <c r="F27" s="7" t="s">
+        <v>275</v>
+      </c>
+    </row>
+    <row r="28" spans="1:6">
+      <c r="A28" s="1" t="s">
+        <v>198</v>
+      </c>
+      <c r="B28" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="C28" s="23">
+        <v>70.070346999999998</v>
+      </c>
+      <c r="D28" s="23">
+        <v>28.016017000000002</v>
+      </c>
+      <c r="E28" s="1" t="s">
         <v>276</v>
       </c>
-    </row>
-    <row r="28" spans="1:6">
-      <c r="A28" s="4" t="s">
-        <v>142</v>
-      </c>
-      <c r="B28" s="4" t="s">
-        <v>143</v>
-      </c>
-      <c r="C28" s="23">
-        <v>70.069685304299611</v>
-      </c>
-      <c r="D28" s="23">
-        <v>27.720222929469681</v>
-      </c>
-      <c r="E28" s="4" t="s">
-        <v>147</v>
-      </c>
-      <c r="F28" s="4" t="s">
-        <v>274</v>
+      <c r="F28" s="1" t="s">
+        <v>283</v>
       </c>
     </row>
     <row r="29" spans="1:6">
       <c r="A29" s="1" t="s">
-        <v>198</v>
+        <v>105</v>
       </c>
       <c r="B29" s="1" t="s">
-        <v>49</v>
+        <v>286</v>
       </c>
       <c r="C29" s="23">
-        <v>70.070346999999998</v>
+        <v>70.074292</v>
       </c>
       <c r="D29" s="23">
-        <v>28.016017000000002</v>
+        <v>27.705573000000001</v>
       </c>
       <c r="E29" s="1" t="s">
-        <v>277</v>
+        <v>284</v>
       </c>
       <c r="F29" s="1" t="s">
-        <v>284</v>
+        <v>285</v>
       </c>
     </row>
     <row r="30" spans="1:6">
       <c r="A30" s="1" t="s">
-        <v>105</v>
+        <v>84</v>
       </c>
       <c r="B30" s="1" t="s">
-        <v>106</v>
+        <v>85</v>
       </c>
       <c r="C30" s="23">
-        <v>70.074292</v>
+        <v>70.166214999999994</v>
       </c>
       <c r="D30" s="23">
-        <v>27.705573000000001</v>
+        <v>28.22343</v>
       </c>
       <c r="E30" s="1" t="s">
         <v>146</v>
       </c>
       <c r="F30" s="1" t="s">
-        <v>272</v>
+        <v>271</v>
       </c>
     </row>
     <row r="31" spans="1:6">
-      <c r="A31" s="1" t="s">
-        <v>84</v>
-      </c>
-      <c r="B31" s="1" t="s">
-        <v>85</v>
+      <c r="A31" s="4" t="s">
+        <v>138</v>
+      </c>
+      <c r="B31" s="4" t="s">
+        <v>139</v>
       </c>
       <c r="C31" s="23">
-        <v>70.166214999999994</v>
+        <v>70.195935132530565</v>
       </c>
       <c r="D31" s="23">
-        <v>28.22343</v>
-      </c>
-      <c r="E31" s="1" t="s">
-        <v>146</v>
-      </c>
-      <c r="F31" s="1" t="s">
-        <v>271</v>
+        <v>28.19830818020764</v>
+      </c>
+      <c r="E31" s="4" t="s">
+        <v>147</v>
+      </c>
+      <c r="F31" s="4" t="s">
+        <v>273</v>
       </c>
     </row>
     <row r="32" spans="1:6">
       <c r="A32" s="4" t="s">
-        <v>138</v>
+        <v>140</v>
       </c>
       <c r="B32" s="4" t="s">
-        <v>139</v>
+        <v>141</v>
       </c>
       <c r="C32" s="23">
-        <v>70.195935132530565</v>
+        <v>70.22968067182029</v>
       </c>
       <c r="D32" s="23">
-        <v>28.19830818020764</v>
+        <v>28.16908580439851</v>
       </c>
       <c r="E32" s="4" t="s">
         <v>147</v>
       </c>
       <c r="F32" s="4" t="s">
-        <v>274</v>
+        <v>273</v>
       </c>
     </row>
     <row r="33" spans="1:6">
-      <c r="A33" s="4" t="s">
-        <v>140</v>
-      </c>
-      <c r="B33" s="4" t="s">
-        <v>141</v>
+      <c r="A33" s="1" t="s">
+        <v>91</v>
+      </c>
+      <c r="B33" s="1" t="s">
+        <v>92</v>
       </c>
       <c r="C33" s="23">
-        <v>70.22968067182029</v>
+        <v>70.375489999999999</v>
       </c>
       <c r="D33" s="23">
-        <v>28.16908580439851</v>
-      </c>
-      <c r="E33" s="4" t="s">
-        <v>147</v>
-      </c>
-      <c r="F33" s="4" t="s">
-        <v>274</v>
+        <v>28.249378</v>
+      </c>
+      <c r="E33" s="1" t="s">
+        <v>146</v>
+      </c>
+      <c r="F33" t="s">
+        <v>266</v>
       </c>
     </row>
     <row r="34" spans="1:6">
       <c r="A34" s="1" t="s">
-        <v>91</v>
+        <v>52</v>
       </c>
       <c r="B34" s="1" t="s">
-        <v>92</v>
+        <v>53</v>
       </c>
       <c r="C34" s="23">
-        <v>70.375489999999999</v>
+        <v>70.419150999999999</v>
       </c>
       <c r="D34" s="23">
-        <v>28.249378</v>
+        <v>28.041376</v>
       </c>
       <c r="E34" s="1" t="s">
         <v>146</v>
       </c>
-      <c r="F34" t="s">
-        <v>266</v>
+      <c r="F34" s="1" t="s">
+        <v>267</v>
       </c>
     </row>
     <row r="35" spans="1:6">
-      <c r="A35" s="1" t="s">
-        <v>52</v>
-      </c>
-      <c r="B35" s="1" t="s">
-        <v>53</v>
-      </c>
-      <c r="C35" s="23">
-        <v>70.419150999999999</v>
-      </c>
-      <c r="D35" s="23">
-        <v>28.041376</v>
+      <c r="A35" s="2" t="s">
+        <v>99</v>
+      </c>
+      <c r="B35" s="2" t="s">
+        <v>100</v>
+      </c>
+      <c r="C35" s="25">
+        <v>70.472215000000006</v>
+      </c>
+      <c r="D35" s="25">
+        <v>28.824532000000001</v>
       </c>
       <c r="E35" s="1" t="s">
         <v>146</v>
       </c>
-      <c r="F35" s="1" t="s">
-        <v>267</v>
-      </c>
-    </row>
-    <row r="36" spans="1:6">
-      <c r="A36" s="2" t="s">
-        <v>99</v>
-      </c>
-      <c r="B36" s="2" t="s">
-        <v>100</v>
-      </c>
-      <c r="C36" s="25">
-        <v>70.472215000000006</v>
-      </c>
-      <c r="D36" s="25">
-        <v>28.824532000000001</v>
-      </c>
-      <c r="E36" s="1" t="s">
-        <v>146</v>
-      </c>
-      <c r="F36" s="2" t="s">
+      <c r="F35" s="2" t="s">
         <v>268</v>
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:F36" xr:uid="{2CF353F4-079D-49EA-982B-68B02FF1D592}">
-    <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:F36">
-      <sortCondition ref="C1:C36"/>
+  <autoFilter ref="A1:F35" xr:uid="{2CF353F4-079D-49EA-982B-68B02FF1D592}">
+    <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:F35">
+      <sortCondition ref="C1:C35"/>
     </sortState>
   </autoFilter>
   <phoneticPr fontId="3" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
-</file>
-
-<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5E17FA22-8B99-4F74-B869-E4F468961C2B}">
-  <sheetPr filterMode="1"/>
-  <dimension ref="A1:J35"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection sqref="A1:F35"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
-  <cols>
-    <col min="8" max="8" width="20.7109375" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="22.5703125" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:10">
-      <c r="A1" t="s">
-        <v>2</v>
-      </c>
-      <c r="B1" t="s">
-        <v>3</v>
-      </c>
-      <c r="C1" t="s">
-        <v>5</v>
-      </c>
-      <c r="D1" t="s">
-        <v>6</v>
-      </c>
-      <c r="E1" t="s">
-        <v>22</v>
-      </c>
-      <c r="F1" t="s">
-        <v>23</v>
-      </c>
-      <c r="G1" t="s">
-        <v>207</v>
-      </c>
-      <c r="H1" t="s">
-        <v>234</v>
-      </c>
-      <c r="I1" t="s">
-        <v>238</v>
-      </c>
-      <c r="J1" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="2" spans="1:10">
-      <c r="A2" t="s">
-        <v>26</v>
-      </c>
-      <c r="B2" t="s">
-        <v>27</v>
-      </c>
-      <c r="C2">
-        <v>1003</v>
-      </c>
-      <c r="D2" t="s">
-        <v>75</v>
-      </c>
-      <c r="E2">
-        <v>24.474238</v>
-      </c>
-      <c r="F2">
-        <v>69.390030999999993</v>
-      </c>
-      <c r="G2">
-        <v>1</v>
-      </c>
-      <c r="H2">
-        <v>1</v>
-      </c>
-      <c r="J2" t="s">
-        <v>61</v>
-      </c>
-    </row>
-    <row r="3" spans="1:10">
-      <c r="A3" t="s">
-        <v>26</v>
-      </c>
-      <c r="B3" t="s">
-        <v>27</v>
-      </c>
-      <c r="C3">
-        <v>1001</v>
-      </c>
-      <c r="D3" t="s">
-        <v>28</v>
-      </c>
-      <c r="E3">
-        <v>24.474238</v>
-      </c>
-      <c r="F3">
-        <v>69.390030999999993</v>
-      </c>
-      <c r="G3">
-        <v>1</v>
-      </c>
-      <c r="H3">
-        <v>1</v>
-      </c>
-      <c r="J3" t="s">
-        <v>61</v>
-      </c>
-    </row>
-    <row r="4" spans="1:10">
-      <c r="A4" t="s">
-        <v>91</v>
-      </c>
-      <c r="B4" t="s">
-        <v>92</v>
-      </c>
-      <c r="C4">
-        <v>2000</v>
-      </c>
-      <c r="D4" t="s">
-        <v>93</v>
-      </c>
-      <c r="E4">
-        <v>28.249378</v>
-      </c>
-      <c r="F4">
-        <v>70.375489999999999</v>
-      </c>
-      <c r="G4">
-        <v>1</v>
-      </c>
-      <c r="H4">
-        <v>1</v>
-      </c>
-      <c r="J4" t="s">
-        <v>97</v>
-      </c>
-    </row>
-    <row r="5" spans="1:10">
-      <c r="A5" t="s">
-        <v>91</v>
-      </c>
-      <c r="B5" t="s">
-        <v>92</v>
-      </c>
-      <c r="C5">
-        <v>2015</v>
-      </c>
-      <c r="D5" t="s">
-        <v>211</v>
-      </c>
-      <c r="E5">
-        <v>28.249378</v>
-      </c>
-      <c r="F5">
-        <v>70.375489999999999</v>
-      </c>
-      <c r="G5">
-        <v>1</v>
-      </c>
-      <c r="H5">
-        <v>1</v>
-      </c>
-      <c r="J5" t="s">
-        <v>97</v>
-      </c>
-    </row>
-    <row r="6" spans="1:10">
-      <c r="A6" t="s">
-        <v>36</v>
-      </c>
-      <c r="B6" t="s">
-        <v>37</v>
-      </c>
-      <c r="C6">
-        <v>1001</v>
-      </c>
-      <c r="D6" t="s">
-        <v>28</v>
-      </c>
-      <c r="E6">
-        <v>24.388183000000001</v>
-      </c>
-      <c r="F6">
-        <v>69.565611000000004</v>
-      </c>
-      <c r="G6">
-        <v>1</v>
-      </c>
-      <c r="H6">
-        <v>1</v>
-      </c>
-      <c r="J6" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="7" spans="1:10">
-      <c r="A7" s="8" t="s">
-        <v>99</v>
-      </c>
-      <c r="B7" s="8" t="s">
-        <v>100</v>
-      </c>
-      <c r="C7" s="8">
-        <v>1001</v>
-      </c>
-      <c r="D7" s="8" t="s">
-        <v>28</v>
-      </c>
-      <c r="E7" s="8">
-        <v>28.824532000000001</v>
-      </c>
-      <c r="F7" s="8">
-        <v>70.472215000000006</v>
-      </c>
-      <c r="G7" s="8">
-        <v>1</v>
-      </c>
-      <c r="H7" s="8">
-        <v>1</v>
-      </c>
-      <c r="I7" s="8"/>
-      <c r="J7" s="8" t="s">
-        <v>103</v>
-      </c>
-    </row>
-    <row r="8" spans="1:10">
-      <c r="A8" s="8" t="s">
-        <v>99</v>
-      </c>
-      <c r="B8" s="8" t="s">
-        <v>100</v>
-      </c>
-      <c r="C8" s="8">
-        <v>1208</v>
-      </c>
-      <c r="D8" s="8" t="s">
-        <v>107</v>
-      </c>
-      <c r="E8" s="8">
-        <v>28.824532000000001</v>
-      </c>
-      <c r="F8" s="8">
-        <v>70.472215000000006</v>
-      </c>
-      <c r="G8" s="8">
-        <v>1</v>
-      </c>
-      <c r="H8" s="8">
-        <v>1</v>
-      </c>
-      <c r="I8" s="8"/>
-      <c r="J8" s="8" t="s">
-        <v>103</v>
-      </c>
-    </row>
-    <row r="9" spans="1:10">
-      <c r="A9" s="8" t="s">
-        <v>99</v>
-      </c>
-      <c r="B9" s="8" t="s">
-        <v>100</v>
-      </c>
-      <c r="C9" s="8">
-        <v>1200</v>
-      </c>
-      <c r="D9" s="8" t="s">
-        <v>215</v>
-      </c>
-      <c r="E9" s="8">
-        <v>28.824532000000001</v>
-      </c>
-      <c r="F9" s="8">
-        <v>70.472215000000006</v>
-      </c>
-      <c r="G9" s="8">
-        <v>1</v>
-      </c>
-      <c r="H9" s="8">
-        <v>1</v>
-      </c>
-      <c r="I9" s="8"/>
-      <c r="J9" s="8" t="s">
-        <v>103</v>
-      </c>
-    </row>
-    <row r="10" spans="1:10">
-      <c r="A10" t="s">
-        <v>66</v>
-      </c>
-      <c r="B10" t="s">
-        <v>67</v>
-      </c>
-      <c r="C10">
-        <v>1000</v>
-      </c>
-      <c r="D10" t="s">
-        <v>68</v>
-      </c>
-      <c r="E10">
-        <v>25.510739000000001</v>
-      </c>
-      <c r="F10">
-        <v>69.469237000000007</v>
-      </c>
-      <c r="G10">
-        <v>1</v>
-      </c>
-      <c r="H10">
-        <v>1</v>
-      </c>
-      <c r="J10" t="s">
-        <v>71</v>
-      </c>
-    </row>
-    <row r="11" spans="1:10">
-      <c r="A11" t="s">
-        <v>66</v>
-      </c>
-      <c r="B11" t="s">
-        <v>67</v>
-      </c>
-      <c r="C11">
-        <v>1003</v>
-      </c>
-      <c r="D11" t="s">
-        <v>75</v>
-      </c>
-      <c r="E11">
-        <v>25.510739000000001</v>
-      </c>
-      <c r="F11">
-        <v>69.469237000000007</v>
-      </c>
-      <c r="G11">
-        <v>1</v>
-      </c>
-      <c r="H11">
-        <v>1</v>
-      </c>
-      <c r="J11" t="s">
-        <v>71</v>
-      </c>
-    </row>
-    <row r="12" spans="1:10" hidden="1">
-      <c r="A12" t="s">
-        <v>201</v>
-      </c>
-      <c r="B12" t="s">
-        <v>202</v>
-      </c>
-      <c r="C12">
-        <v>2000</v>
-      </c>
-      <c r="D12" t="s">
-        <v>93</v>
-      </c>
-      <c r="E12">
-        <v>25.815045999999999</v>
-      </c>
-      <c r="F12">
-        <v>69.400755000000004</v>
-      </c>
-      <c r="G12">
-        <v>1</v>
-      </c>
-      <c r="H12">
-        <v>0</v>
-      </c>
-      <c r="J12" t="s">
-        <v>235</v>
-      </c>
-    </row>
-    <row r="13" spans="1:10" hidden="1">
-      <c r="A13" t="s">
-        <v>201</v>
-      </c>
-      <c r="B13" t="s">
-        <v>202</v>
-      </c>
-      <c r="C13">
-        <v>2015</v>
-      </c>
-      <c r="D13" t="s">
-        <v>211</v>
-      </c>
-      <c r="E13">
-        <v>25.815045999999999</v>
-      </c>
-      <c r="F13">
-        <v>69.400755000000004</v>
-      </c>
-      <c r="G13">
-        <v>1</v>
-      </c>
-      <c r="H13">
-        <v>0</v>
-      </c>
-      <c r="J13" t="s">
-        <v>235</v>
-      </c>
-    </row>
-    <row r="14" spans="1:10" hidden="1">
-      <c r="A14" t="s">
-        <v>203</v>
-      </c>
-      <c r="B14" t="s">
-        <v>204</v>
-      </c>
-      <c r="C14">
-        <v>2000</v>
-      </c>
-      <c r="D14" t="s">
-        <v>93</v>
-      </c>
-      <c r="E14">
-        <v>25.814402000000001</v>
-      </c>
-      <c r="F14">
-        <v>69.400858999999997</v>
-      </c>
-      <c r="G14">
-        <v>1</v>
-      </c>
-      <c r="H14">
-        <v>0</v>
-      </c>
-      <c r="J14" t="s">
-        <v>235</v>
-      </c>
-    </row>
-    <row r="15" spans="1:10">
-      <c r="A15" t="s">
-        <v>205</v>
-      </c>
-      <c r="B15" t="s">
-        <v>206</v>
-      </c>
-      <c r="C15">
-        <v>2006</v>
-      </c>
-      <c r="D15" t="s">
-        <v>209</v>
-      </c>
-      <c r="E15">
-        <v>25.814402000000001</v>
-      </c>
-      <c r="F15">
-        <v>69.400858999999997</v>
-      </c>
-      <c r="G15">
-        <v>1</v>
-      </c>
-      <c r="H15">
-        <v>1</v>
-      </c>
-      <c r="J15" t="s">
-        <v>235</v>
-      </c>
-    </row>
-    <row r="16" spans="1:10">
-      <c r="A16" t="s">
-        <v>205</v>
-      </c>
-      <c r="B16" t="s">
-        <v>206</v>
-      </c>
-      <c r="C16">
-        <v>2015</v>
-      </c>
-      <c r="D16" t="s">
-        <v>211</v>
-      </c>
-      <c r="E16">
-        <v>25.814402000000001</v>
-      </c>
-      <c r="F16">
-        <v>69.400858999999997</v>
-      </c>
-      <c r="G16">
-        <v>1</v>
-      </c>
-      <c r="H16">
-        <v>1</v>
-      </c>
-      <c r="J16" t="s">
-        <v>235</v>
-      </c>
-    </row>
-    <row r="17" spans="1:10">
-      <c r="A17" t="s">
-        <v>205</v>
-      </c>
-      <c r="B17" t="s">
-        <v>206</v>
-      </c>
-      <c r="C17">
-        <v>2001</v>
-      </c>
-      <c r="D17" t="s">
-        <v>216</v>
-      </c>
-      <c r="E17">
-        <v>25.814402000000001</v>
-      </c>
-      <c r="F17">
-        <v>69.400858999999997</v>
-      </c>
-      <c r="G17">
-        <v>1</v>
-      </c>
-      <c r="H17">
-        <v>1</v>
-      </c>
-      <c r="J17" t="s">
-        <v>235</v>
-      </c>
-    </row>
-    <row r="18" spans="1:10">
-      <c r="A18" t="s">
-        <v>205</v>
-      </c>
-      <c r="B18" t="s">
-        <v>206</v>
-      </c>
-      <c r="C18">
-        <v>2000</v>
-      </c>
-      <c r="D18" t="s">
-        <v>93</v>
-      </c>
-      <c r="E18">
-        <v>25.814402000000001</v>
-      </c>
-      <c r="F18">
-        <v>69.400858999999997</v>
-      </c>
-      <c r="G18">
-        <v>1</v>
-      </c>
-      <c r="H18">
-        <v>1</v>
-      </c>
-      <c r="J18" t="s">
-        <v>235</v>
-      </c>
-    </row>
-    <row r="19" spans="1:10">
-      <c r="A19" t="s">
-        <v>78</v>
-      </c>
-      <c r="B19" t="s">
-        <v>79</v>
-      </c>
-      <c r="C19">
-        <v>1000</v>
-      </c>
-      <c r="D19" t="s">
-        <v>68</v>
-      </c>
-      <c r="E19">
-        <v>26.485793000000001</v>
-      </c>
-      <c r="F19">
-        <v>69.944618000000006</v>
-      </c>
-      <c r="G19">
-        <v>1</v>
-      </c>
-      <c r="H19">
-        <v>1</v>
-      </c>
-      <c r="J19" t="s">
-        <v>81</v>
-      </c>
-    </row>
-    <row r="20" spans="1:10">
-      <c r="A20" t="s">
-        <v>42</v>
-      </c>
-      <c r="B20" t="s">
-        <v>43</v>
-      </c>
-      <c r="C20">
-        <v>1001</v>
-      </c>
-      <c r="D20" t="s">
-        <v>28</v>
-      </c>
-      <c r="E20">
-        <v>25.158322999999999</v>
-      </c>
-      <c r="F20">
-        <v>69.419317000000007</v>
-      </c>
-      <c r="G20">
-        <v>1</v>
-      </c>
-      <c r="H20">
-        <v>1</v>
-      </c>
-      <c r="J20" t="s">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="21" spans="1:10" hidden="1">
-      <c r="A21" t="s">
-        <v>197</v>
-      </c>
-      <c r="B21" t="s">
-        <v>198</v>
-      </c>
-      <c r="C21">
-        <v>1001</v>
-      </c>
-      <c r="D21" t="s">
-        <v>28</v>
-      </c>
-      <c r="E21">
-        <v>28.057406</v>
-      </c>
-      <c r="F21">
-        <v>70.072616999999994</v>
-      </c>
-      <c r="G21">
-        <v>1</v>
-      </c>
-      <c r="H21">
-        <v>0</v>
-      </c>
-      <c r="I21" t="s">
-        <v>48</v>
-      </c>
-      <c r="J21" t="s">
-        <v>229</v>
-      </c>
-    </row>
-    <row r="22" spans="1:10">
-      <c r="A22" t="s">
-        <v>48</v>
-      </c>
-      <c r="B22" t="s">
-        <v>49</v>
-      </c>
-      <c r="C22">
-        <v>1200</v>
-      </c>
-      <c r="D22" t="s">
-        <v>215</v>
-      </c>
-      <c r="E22">
-        <v>28.016017000000002</v>
-      </c>
-      <c r="F22">
-        <v>70.070346999999998</v>
-      </c>
-      <c r="G22">
-        <v>1</v>
-      </c>
-      <c r="H22">
-        <v>1</v>
-      </c>
-      <c r="J22" t="s">
-        <v>82</v>
-      </c>
-    </row>
-    <row r="23" spans="1:10">
-      <c r="A23" t="s">
-        <v>48</v>
-      </c>
-      <c r="B23" t="s">
-        <v>49</v>
-      </c>
-      <c r="C23">
-        <v>1208</v>
-      </c>
-      <c r="D23" t="s">
-        <v>107</v>
-      </c>
-      <c r="E23">
-        <v>28.016017000000002</v>
-      </c>
-      <c r="F23">
-        <v>70.070346999999998</v>
-      </c>
-      <c r="G23">
-        <v>1</v>
-      </c>
-      <c r="H23">
-        <v>1</v>
-      </c>
-      <c r="J23" t="s">
-        <v>82</v>
-      </c>
-    </row>
-    <row r="24" spans="1:10">
-      <c r="A24" t="s">
-        <v>48</v>
-      </c>
-      <c r="B24" t="s">
-        <v>49</v>
-      </c>
-      <c r="C24">
-        <v>1001</v>
-      </c>
-      <c r="D24" t="s">
-        <v>28</v>
-      </c>
-      <c r="E24">
-        <v>28.016017000000002</v>
-      </c>
-      <c r="F24">
-        <v>70.070346999999998</v>
-      </c>
-      <c r="G24">
-        <v>1</v>
-      </c>
-      <c r="H24">
-        <v>1</v>
-      </c>
-      <c r="J24" t="s">
-        <v>82</v>
-      </c>
-    </row>
-    <row r="25" spans="1:10">
-      <c r="A25" t="s">
-        <v>48</v>
-      </c>
-      <c r="B25" t="s">
-        <v>49</v>
-      </c>
-      <c r="C25">
-        <v>1003</v>
-      </c>
-      <c r="D25" t="s">
-        <v>75</v>
-      </c>
-      <c r="E25">
-        <v>28.016017000000002</v>
-      </c>
-      <c r="F25">
-        <v>70.070346999999998</v>
-      </c>
-      <c r="G25">
-        <v>1</v>
-      </c>
-      <c r="H25">
-        <v>1</v>
-      </c>
-      <c r="J25" t="s">
-        <v>82</v>
-      </c>
-    </row>
-    <row r="26" spans="1:10">
-      <c r="A26" t="s">
-        <v>84</v>
-      </c>
-      <c r="B26" t="s">
-        <v>85</v>
-      </c>
-      <c r="C26">
-        <v>2002</v>
-      </c>
-      <c r="D26" t="s">
-        <v>214</v>
-      </c>
-      <c r="E26">
-        <v>28.22343</v>
-      </c>
-      <c r="F26">
-        <v>70.166214999999994</v>
-      </c>
-      <c r="G26">
-        <v>1</v>
-      </c>
-      <c r="H26">
-        <v>1</v>
-      </c>
-      <c r="J26" t="s">
-        <v>88</v>
-      </c>
-    </row>
-    <row r="27" spans="1:10">
-      <c r="A27" t="s">
-        <v>52</v>
-      </c>
-      <c r="B27" t="s">
-        <v>53</v>
-      </c>
-      <c r="C27">
-        <v>1001</v>
-      </c>
-      <c r="D27" t="s">
-        <v>28</v>
-      </c>
-      <c r="E27">
-        <v>28.041376</v>
-      </c>
-      <c r="F27">
-        <v>70.419150999999999</v>
-      </c>
-      <c r="G27">
-        <v>1</v>
-      </c>
-      <c r="H27">
-        <v>1</v>
-      </c>
-      <c r="J27" t="s">
-        <v>89</v>
-      </c>
-    </row>
-    <row r="28" spans="1:10" hidden="1">
-      <c r="A28" t="s">
-        <v>217</v>
-      </c>
-      <c r="B28" t="s">
-        <v>218</v>
-      </c>
-      <c r="C28">
-        <v>1003</v>
-      </c>
-      <c r="D28" t="s">
-        <v>75</v>
-      </c>
-      <c r="E28">
-        <v>27.78257</v>
-      </c>
-      <c r="F28">
-        <v>70.070637000000005</v>
-      </c>
-      <c r="G28">
-        <v>1</v>
-      </c>
-      <c r="H28">
-        <v>0</v>
-      </c>
-      <c r="I28" t="s">
-        <v>105</v>
-      </c>
-      <c r="J28" t="s">
-        <v>237</v>
-      </c>
-    </row>
-    <row r="29" spans="1:10" hidden="1">
-      <c r="A29" t="s">
-        <v>219</v>
-      </c>
-      <c r="B29" t="s">
-        <v>220</v>
-      </c>
-      <c r="C29">
-        <v>1003</v>
-      </c>
-      <c r="D29" t="s">
-        <v>75</v>
-      </c>
-      <c r="E29">
-        <v>28.055733</v>
-      </c>
-      <c r="F29">
-        <v>70.072055000000006</v>
-      </c>
-      <c r="G29">
-        <v>1</v>
-      </c>
-      <c r="H29">
-        <v>0</v>
-      </c>
-      <c r="I29" t="s">
-        <v>48</v>
-      </c>
-      <c r="J29" t="s">
-        <v>239</v>
-      </c>
-    </row>
-    <row r="30" spans="1:10">
-      <c r="A30" t="s">
-        <v>105</v>
-      </c>
-      <c r="B30" t="s">
-        <v>106</v>
-      </c>
-      <c r="C30">
-        <v>1200</v>
-      </c>
-      <c r="D30" t="s">
-        <v>215</v>
-      </c>
-      <c r="E30">
-        <v>27.705573000000001</v>
-      </c>
-      <c r="F30">
-        <v>70.074292</v>
-      </c>
-      <c r="G30">
-        <v>1</v>
-      </c>
-      <c r="H30">
-        <v>1</v>
-      </c>
-      <c r="J30" t="s">
-        <v>108</v>
-      </c>
-    </row>
-    <row r="31" spans="1:10">
-      <c r="A31" t="s">
-        <v>105</v>
-      </c>
-      <c r="B31" t="s">
-        <v>106</v>
-      </c>
-      <c r="C31">
-        <v>1208</v>
-      </c>
-      <c r="D31" t="s">
-        <v>107</v>
-      </c>
-      <c r="E31">
-        <v>27.705573000000001</v>
-      </c>
-      <c r="F31">
-        <v>70.074292</v>
-      </c>
-      <c r="G31">
-        <v>1</v>
-      </c>
-      <c r="H31">
-        <v>1</v>
-      </c>
-      <c r="J31" t="s">
-        <v>108</v>
-      </c>
-    </row>
-    <row r="32" spans="1:10">
-      <c r="A32" t="s">
-        <v>57</v>
-      </c>
-      <c r="B32" t="s">
-        <v>58</v>
-      </c>
-      <c r="C32">
-        <v>1001</v>
-      </c>
-      <c r="D32" t="s">
-        <v>28</v>
-      </c>
-      <c r="E32">
-        <v>24.938338000000002</v>
-      </c>
-      <c r="F32">
-        <v>69.426393000000004</v>
-      </c>
-      <c r="G32">
-        <v>1</v>
-      </c>
-      <c r="H32">
-        <v>1</v>
-      </c>
-      <c r="J32" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="33" spans="1:10">
-      <c r="A33" t="s">
-        <v>57</v>
-      </c>
-      <c r="B33" t="s">
-        <v>58</v>
-      </c>
-      <c r="C33">
-        <v>1003</v>
-      </c>
-      <c r="D33" t="s">
-        <v>75</v>
-      </c>
-      <c r="E33">
-        <v>24.938338000000002</v>
-      </c>
-      <c r="F33">
-        <v>69.426393000000004</v>
-      </c>
-      <c r="G33">
-        <v>1</v>
-      </c>
-      <c r="H33">
-        <v>1</v>
-      </c>
-      <c r="J33" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="34" spans="1:10" hidden="1">
-      <c r="A34" t="s">
-        <v>199</v>
-      </c>
-      <c r="B34" t="s">
-        <v>200</v>
-      </c>
-      <c r="C34">
-        <v>1001</v>
-      </c>
-      <c r="D34" t="s">
-        <v>28</v>
-      </c>
-      <c r="E34">
-        <v>24.945211</v>
-      </c>
-      <c r="F34">
-        <v>69.427194</v>
-      </c>
-      <c r="G34">
-        <v>1</v>
-      </c>
-      <c r="H34">
-        <v>0</v>
-      </c>
-      <c r="I34" t="s">
-        <v>57</v>
-      </c>
-      <c r="J34" t="s">
-        <v>233</v>
-      </c>
-    </row>
-    <row r="35" spans="1:10">
-      <c r="A35" t="s">
-        <v>73</v>
-      </c>
-      <c r="B35" t="s">
-        <v>74</v>
-      </c>
-      <c r="C35">
-        <v>2000</v>
-      </c>
-      <c r="D35" t="s">
-        <v>93</v>
-      </c>
-      <c r="E35">
-        <v>25.811848999999999</v>
-      </c>
-      <c r="F35">
-        <v>69.408237</v>
-      </c>
-      <c r="G35">
-        <v>1</v>
-      </c>
-      <c r="H35">
-        <v>1</v>
-      </c>
-      <c r="J35" t="s">
-        <v>236</v>
-      </c>
-    </row>
-  </sheetData>
-  <autoFilter ref="A1:AB35" xr:uid="{FFFD35B6-2FA8-40AC-A5C6-3E4817891152}">
-    <filterColumn colId="7">
-      <filters>
-        <filter val="1"/>
-      </filters>
-    </filterColumn>
-  </autoFilter>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
 </file>
</xml_diff>